<commit_message>
Update 2020-03-18 22:12 New Charts
</commit_message>
<xml_diff>
--- a/COVID-19 Apps/Growth Chart.xlsx
+++ b/COVID-19 Apps/Growth Chart.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zur Bonsen Georg\Documents\Programme\Beyond4P_Apps\COVID-19 Apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D14F976-0BF3-41AE-B9B9-105B4000A549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A33A65-A1A6-48FA-881C-6565E1EBEF51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{A4C1FE6B-DE9B-48BC-897C-015B097916DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{A4C1FE6B-DE9B-48BC-897C-015B097916DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="TABLE" sheetId="1" r:id="rId1"/>
+    <sheet name="CHART" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Country/Region</t>
   </si>
@@ -86,36 +87,6 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>Flat curve:</t>
-  </si>
-  <si>
-    <t>Declining:</t>
-  </si>
-  <si>
-    <t>Growth is no longer exponential</t>
-  </si>
-  <si>
-    <t>Inreasing:</t>
-  </si>
-  <si>
-    <t>Growth is worse than exponential</t>
-  </si>
-  <si>
-    <t>Growth is at same percentage from day to day (actually exponential growth on linear scale)</t>
-  </si>
-  <si>
-    <t>No growth anymore.  China is a good example.  Followed by Korea</t>
-  </si>
-  <si>
-    <t>Target:</t>
-  </si>
-  <si>
-    <t>All countries should sooner or later reache a plain zero</t>
-  </si>
-  <si>
-    <t>Algorithm</t>
-  </si>
-  <si>
     <t>Day 1</t>
   </si>
   <si>
@@ -145,12 +116,66 @@
   <si>
     <t>on day to day base</t>
   </si>
+  <si>
+    <t>Curve at or near 0%:</t>
+  </si>
+  <si>
+    <t>Very successful with containment measures</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Country (example)</t>
+  </si>
+  <si>
+    <t>&lt;8%, decreasing:</t>
+  </si>
+  <si>
+    <t>New infections typ. smaller than recoveries.  Active cases decreasing.</t>
+  </si>
+  <si>
+    <t>S. Korea</t>
+  </si>
+  <si>
+    <t>&gt;8%, decreasing:</t>
+  </si>
+  <si>
+    <t>Number of infections are increasing, but sub-exponentially</t>
+  </si>
+  <si>
+    <t>&gt;8%, constant:</t>
+  </si>
+  <si>
+    <t>Number of infections increase exponentially</t>
+  </si>
+  <si>
+    <t>&gt;8%, increasing:</t>
+  </si>
+  <si>
+    <t>Number of infactions increase above exponential curve</t>
+  </si>
+  <si>
+    <t>Calculation method:</t>
+  </si>
+  <si>
+    <t>Compound Averae growth on daily base spanning over 7 days:</t>
+  </si>
+  <si>
+    <t>Average of last 3 days are compared with average of beginning 3 days.</t>
+  </si>
+  <si>
+    <t>This algorithm smoothens out short term discontinuities, e.g. reporting outages or peaks</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +186,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -238,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -248,6 +281,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -357,7 +392,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$2</c:f>
+              <c:f>TABLE!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -380,120 +415,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$R$2</c:f>
+              <c:f>TABLE!$B$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.65490000000000004</c:v>
+                  <c:v>0.59670000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59670000000000001</c:v>
+                  <c:v>0.55569999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55569999999999997</c:v>
+                  <c:v>0.60429999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60429999999999995</c:v>
+                  <c:v>0.4592</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4592</c:v>
+                  <c:v>0.36780000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.32140000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.36780000000000002</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.32140000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.34799999999999998</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36780000000000002</c:v>
+                  <c:v>0.3629</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3629</c:v>
+                  <c:v>0.35149999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.35149999999999998</c:v>
+                  <c:v>0.33689999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.33689999999999998</c:v>
+                  <c:v>0.32340000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.32340000000000002</c:v>
+                  <c:v>0.35289999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.35289999999999999</c:v>
+                  <c:v>0.36809999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.36809999999999998</c:v>
+                  <c:v>0.37859999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.37859999999999999</c:v>
+                  <c:v>0.36480000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.36480000000000001</c:v>
+                  <c:v>0.32169999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,7 +536,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000000-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -510,7 +545,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$3</c:f>
+              <c:f>TABLE!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -533,120 +568,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$R$3</c:f>
+              <c:f>TABLE!$B$3:$R$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7.46E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.46E-2</c:v>
+                  <c:v>0.38379999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38379999999999997</c:v>
+                  <c:v>0.66400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66400000000000003</c:v>
+                  <c:v>0.95699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95699999999999996</c:v>
+                  <c:v>1.1533</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1533</c:v>
+                  <c:v>1.0167999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0167999999999999</c:v>
+                  <c:v>0.94330000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.94330000000000003</c:v>
+                  <c:v>0.8155</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8155</c:v>
+                  <c:v>0.63060000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.63060000000000005</c:v>
+                  <c:v>0.40339999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.40339999999999998</c:v>
+                  <c:v>0.25740000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.25740000000000002</c:v>
+                  <c:v>0.16980000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16980000000000001</c:v>
+                  <c:v>0.18210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.18210000000000001</c:v>
+                  <c:v>0.21959999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.21959999999999999</c:v>
+                  <c:v>0.27010000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.27010000000000001</c:v>
+                  <c:v>0.30969999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.30969999999999998</c:v>
+                  <c:v>0.28010000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -654,7 +689,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000001-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -663,7 +698,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$4</c:f>
+              <c:f>TABLE!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -686,120 +721,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$R$4</c:f>
+              <c:f>TABLE!$B$4:$R$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.1188</c:v>
+                  <c:v>0.1603</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1603</c:v>
+                  <c:v>0.19339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19339999999999999</c:v>
+                  <c:v>0.20830000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20830000000000001</c:v>
+                  <c:v>0.17630000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17630000000000001</c:v>
+                  <c:v>0.1459</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1459</c:v>
+                  <c:v>0.13780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13780000000000001</c:v>
+                  <c:v>0.14660000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14660000000000001</c:v>
+                  <c:v>0.1671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1671</c:v>
+                  <c:v>0.1817</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1817</c:v>
+                  <c:v>0.1661</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1661</c:v>
+                  <c:v>0.17180000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.17180000000000001</c:v>
+                  <c:v>0.16159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16159999999999999</c:v>
+                  <c:v>0.20860000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.20860000000000001</c:v>
+                  <c:v>0.2303</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.2303</c:v>
+                  <c:v>0.24629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.24629999999999999</c:v>
+                  <c:v>0.29649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.29649999999999999</c:v>
+                  <c:v>0.28460000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -807,7 +842,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000002-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -816,7 +851,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$5</c:f>
+              <c:f>TABLE!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -839,111 +874,111 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$5:$R$5</c:f>
+              <c:f>TABLE!$B$5:$R$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>5.4000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5.1999999999999998E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.4000000000000003E-3</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1999999999999998E-3</c:v>
+                  <c:v>4.8999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8999999999999998E-3</c:v>
+                  <c:v>4.1000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1000000000000003E-3</c:v>
+                  <c:v>3.0999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0999999999999999E-3</c:v>
+                  <c:v>2.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3E-3</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6999999999999999E-3</c:v>
+                  <c:v>1.6000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6000000000000001E-3</c:v>
+                  <c:v>1.2999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2999999999999999E-3</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1E-3</c:v>
+                  <c:v>6.9999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.9999999999999999E-4</c:v>
+                  <c:v>5.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.0000000000000001E-4</c:v>
+                  <c:v>4.0000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.0000000000000002E-4</c:v>
+                  <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>2.9999999999999997E-4</c:v>
@@ -960,7 +995,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000003-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -969,7 +1004,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$6</c:f>
+              <c:f>TABLE!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -993,120 +1028,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$6:$R$6</c:f>
+              <c:f>TABLE!$B$6:$R$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.50509999999999999</c:v>
+                  <c:v>0.59809999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59809999999999997</c:v>
+                  <c:v>0.56599999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56599999999999995</c:v>
+                  <c:v>0.46810000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46810000000000002</c:v>
+                  <c:v>0.36799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36799999999999999</c:v>
+                  <c:v>0.32029999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32029999999999997</c:v>
+                  <c:v>0.33169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.33169999999999999</c:v>
+                  <c:v>0.39579999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39579999999999999</c:v>
+                  <c:v>0.41620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.41620000000000001</c:v>
+                  <c:v>0.39560000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.39560000000000001</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33</c:v>
+                  <c:v>0.27689999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27689999999999998</c:v>
+                  <c:v>0.2341</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.23400000000000001</c:v>
+                  <c:v>0.25700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.25669999999999998</c:v>
+                  <c:v>0.26040000000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.26</c:v>
+                  <c:v>0.24390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.24340000000000001</c:v>
+                  <c:v>0.25240000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.25180000000000002</c:v>
+                  <c:v>0.2298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1114,7 +1149,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000004-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1123,7 +1158,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$7</c:f>
+              <c:f>TABLE!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1146,120 +1181,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$7:$R$7</c:f>
+              <c:f>TABLE!$B$7:$R$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.37080000000000002</c:v>
+                  <c:v>0.43859999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43859999999999999</c:v>
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42199999999999999</c:v>
+                  <c:v>0.41489999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41489999999999999</c:v>
+                  <c:v>0.37419999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37419999999999998</c:v>
+                  <c:v>0.38290000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38290000000000002</c:v>
+                  <c:v>0.40010000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.40010000000000001</c:v>
+                  <c:v>0.41620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.41620000000000001</c:v>
+                  <c:v>0.42009999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.42009999999999997</c:v>
+                  <c:v>0.33829999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33829999999999999</c:v>
+                  <c:v>0.26950000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.26950000000000002</c:v>
+                  <c:v>0.23519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.23519999999999999</c:v>
+                  <c:v>0.21360000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.21360000000000001</c:v>
+                  <c:v>0.2626</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2626</c:v>
+                  <c:v>0.29530000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.29530000000000001</c:v>
+                  <c:v>0.32640000000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.32640000000000002</c:v>
+                  <c:v>0.34200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.34200000000000003</c:v>
+                  <c:v>0.30649999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1267,7 +1302,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000005-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1276,7 +1311,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$8</c:f>
+              <c:f>TABLE!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1299,67 +1334,67 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$8:$R$8</c:f>
+              <c:f>TABLE!$B$8:$R$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1367,52 +1402,52 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.1400000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1400000000000001E-2</c:v>
+                  <c:v>9.6299999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6299999999999997E-2</c:v>
+                  <c:v>0.4335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4335</c:v>
+                  <c:v>0.62660000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.62660000000000005</c:v>
+                  <c:v>0.68659999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.68659999999999999</c:v>
+                  <c:v>0.64419999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.64419999999999999</c:v>
+                  <c:v>0.28620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.28620000000000001</c:v>
+                  <c:v>0.16489999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.16489999999999999</c:v>
+                  <c:v>0.1159</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1159</c:v>
+                  <c:v>0.14099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.14099999999999999</c:v>
+                  <c:v>0.1641</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1641</c:v>
+                  <c:v>0.16950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.16950000000000001</c:v>
+                  <c:v>0.16819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.16819999999999999</c:v>
+                  <c:v>0.16539999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.16539999999999999</c:v>
+                  <c:v>0.14990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.14990000000000001</c:v>
+                  <c:v>0.14580000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1420,7 +1455,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000006-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1429,7 +1464,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$9</c:f>
+              <c:f>TABLE!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1454,120 +1489,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$9:$R$9</c:f>
+              <c:f>TABLE!$B$9:$R$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.57550000000000001</c:v>
+                  <c:v>0.60529999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60529999999999995</c:v>
+                  <c:v>0.59140000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59140000000000004</c:v>
+                  <c:v>0.58030000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58030000000000004</c:v>
+                  <c:v>0.5323</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5323</c:v>
+                  <c:v>0.4546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4546</c:v>
+                  <c:v>0.38129999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.38129999999999997</c:v>
+                  <c:v>0.30769999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.30769999999999997</c:v>
+                  <c:v>0.26179999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.26179999999999998</c:v>
+                  <c:v>0.22189999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22189999999999999</c:v>
+                  <c:v>0.1812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1812</c:v>
+                  <c:v>0.14499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.14499999999999999</c:v>
+                  <c:v>0.1216</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1216</c:v>
+                  <c:v>0.11700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11700000000000001</c:v>
+                  <c:v>0.1193</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1193</c:v>
+                  <c:v>0.1196</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1196</c:v>
+                  <c:v>0.1133</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1133</c:v>
+                  <c:v>0.1033</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1575,7 +1610,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000007-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1584,7 +1619,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$10</c:f>
+              <c:f>TABLE!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1607,120 +1642,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$10:$R$10</c:f>
+              <c:f>TABLE!$B$10:$R$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.3947</c:v>
+                  <c:v>0.38650000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38650000000000001</c:v>
+                  <c:v>0.35759999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35759999999999997</c:v>
+                  <c:v>0.32929999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32929999999999998</c:v>
+                  <c:v>0.2999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2999</c:v>
+                  <c:v>0.26329999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26329999999999998</c:v>
+                  <c:v>0.24260000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24260000000000001</c:v>
+                  <c:v>0.2324</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2324</c:v>
+                  <c:v>0.23760000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.23760000000000001</c:v>
+                  <c:v>0.24129999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.24129999999999999</c:v>
+                  <c:v>0.2321</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2321</c:v>
+                  <c:v>0.21940000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.21940000000000001</c:v>
+                  <c:v>0.1832</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1832</c:v>
+                  <c:v>0.17380000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.17380000000000001</c:v>
+                  <c:v>0.17730000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.17730000000000001</c:v>
+                  <c:v>0.18920000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.18920000000000001</c:v>
+                  <c:v>0.20469999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.20469999999999999</c:v>
+                  <c:v>0.18590000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1728,7 +1763,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000008-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1737,7 +1772,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$11</c:f>
+              <c:f>TABLE!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1762,120 +1797,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$11:$R$11</c:f>
+              <c:f>TABLE!$B$11:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.31680000000000003</c:v>
+                  <c:v>0.31640000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31640000000000001</c:v>
+                  <c:v>0.29389999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29389999999999999</c:v>
+                  <c:v>0.25380000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25380000000000003</c:v>
+                  <c:v>0.20200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20200000000000001</c:v>
+                  <c:v>0.16339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16339999999999999</c:v>
+                  <c:v>0.13009999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13009999999999999</c:v>
+                  <c:v>0.10440000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10440000000000001</c:v>
+                  <c:v>8.4500000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.4500000000000006E-2</c:v>
+                  <c:v>6.6199999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.6199999999999995E-2</c:v>
+                  <c:v>5.0700000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0700000000000002E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.6299999999999999E-2</c:v>
+                  <c:v>2.52E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.52E-2</c:v>
+                  <c:v>1.9699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9699999999999999E-2</c:v>
+                  <c:v>1.78E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.78E-2</c:v>
+                  <c:v>1.5900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.5900000000000001E-2</c:v>
+                  <c:v>1.4200000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.4200000000000001E-2</c:v>
+                  <c:v>1.1599999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1883,7 +1918,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{00000009-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1892,7 +1927,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$12</c:f>
+              <c:f>TABLE!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1918,120 +1953,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$12:$R$12</c:f>
+              <c:f>TABLE!$B$12:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.74160000000000004</c:v>
+                  <c:v>0.66400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66400000000000003</c:v>
+                  <c:v>0.64510000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64510000000000001</c:v>
+                  <c:v>0.57479999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57479999999999998</c:v>
+                  <c:v>0.53220000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53220000000000001</c:v>
+                  <c:v>0.4153</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4153</c:v>
+                  <c:v>0.3715</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3715</c:v>
+                  <c:v>0.33129999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33129999999999998</c:v>
+                  <c:v>0.32719999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32719999999999999</c:v>
+                  <c:v>0.36549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36549999999999999</c:v>
+                  <c:v>0.40579999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.40579999999999999</c:v>
+                  <c:v>0.44440000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.44440000000000002</c:v>
+                  <c:v>0.4118</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.4118</c:v>
+                  <c:v>0.44479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.44479999999999997</c:v>
+                  <c:v>0.41770000000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.41770000000000002</c:v>
+                  <c:v>0.4007</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.4007</c:v>
+                  <c:v>0.40179999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.40179999999999999</c:v>
+                  <c:v>0.3175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2039,7 +2074,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{0000000A-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2048,7 +2083,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$13</c:f>
+              <c:f>TABLE!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2071,120 +2106,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$13:$R$13</c:f>
+              <c:f>TABLE!$B$13:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.71579999999999999</c:v>
+                  <c:v>0.69479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69479999999999997</c:v>
+                  <c:v>0.42299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42299999999999999</c:v>
+                  <c:v>0.3296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3296</c:v>
+                  <c:v>0.28549999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28549999999999998</c:v>
+                  <c:v>0.46010000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46010000000000001</c:v>
+                  <c:v>0.53900000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.53900000000000003</c:v>
+                  <c:v>0.63349999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63349999999999995</c:v>
+                  <c:v>0.59970000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.59970000000000001</c:v>
+                  <c:v>0.42120000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.42120000000000002</c:v>
+                  <c:v>0.36820000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.36820000000000003</c:v>
+                  <c:v>0.32669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32669999999999999</c:v>
+                  <c:v>0.32979999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.32979999999999998</c:v>
+                  <c:v>0.32969999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.32969999999999999</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.31</c:v>
+                  <c:v>0.26190000000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.26190000000000002</c:v>
+                  <c:v>0.20699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.20699999999999999</c:v>
+                  <c:v>0.14729999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2192,7 +2227,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{0000000B-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2201,7 +2236,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$14</c:f>
+              <c:f>TABLE!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2228,120 +2263,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$14:$R$14</c:f>
+              <c:f>TABLE!$B$14:$R$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.4147000000000001</c:v>
+                  <c:v>1.2688999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2688999999999999</c:v>
+                  <c:v>0.71740000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71740000000000004</c:v>
+                  <c:v>0.64670000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64670000000000005</c:v>
+                  <c:v>0.53349999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53349999999999997</c:v>
+                  <c:v>0.48820000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48820000000000002</c:v>
+                  <c:v>0.48049999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.48049999999999998</c:v>
+                  <c:v>0.47770000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47770000000000001</c:v>
+                  <c:v>0.44469999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.44469999999999998</c:v>
+                  <c:v>0.39300000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.39300000000000002</c:v>
+                  <c:v>0.30220000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30220000000000002</c:v>
+                  <c:v>0.2631</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2631</c:v>
+                  <c:v>0.2167</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2167</c:v>
+                  <c:v>0.25690000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.25690000000000002</c:v>
+                  <c:v>0.27229999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.27229999999999999</c:v>
+                  <c:v>0.3266</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.3266</c:v>
+                  <c:v>0.33839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.33839999999999998</c:v>
+                  <c:v>0.30570000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2349,7 +2384,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{0000000C-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2358,7 +2393,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$15</c:f>
+              <c:f>TABLE!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2385,67 +2420,67 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$15:$R$15</c:f>
+              <c:f>TABLE!$B$15:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2489,16 +2524,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.63460000000000005</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00%">
-                  <c:v>0.63460000000000005</c:v>
+                  <c:v>0.40489999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00%">
-                  <c:v>0.40489999999999998</c:v>
+                  <c:v>0.30259999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00%">
-                  <c:v>0.30259999999999998</c:v>
+                  <c:v>0.30669999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2506,7 +2541,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{0000000D-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2515,7 +2550,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$A$16</c:f>
+              <c:f>TABLE!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2541,117 +2576,120 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$R$1</c:f>
+              <c:f>TABLE!$B$1:$R$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43890</c:v>
+                  <c:v>43891</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$16:$R$16</c:f>
+              <c:f>TABLE!$B$16:$R$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.1346</c:v>
+                  <c:v>0.193</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.193</c:v>
+                  <c:v>0.24660000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.24660000000000001</c:v>
+                  <c:v>0.27539999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27539999999999998</c:v>
+                  <c:v>0.32169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32169999999999999</c:v>
+                  <c:v>0.3377</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3377</c:v>
+                  <c:v>0.3866</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39939999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39939999999999998</c:v>
+                  <c:v>0.38159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.38159999999999999</c:v>
+                  <c:v>0.3347</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3347</c:v>
+                  <c:v>0.2792</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2792</c:v>
+                  <c:v>0.2437</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2437</c:v>
+                  <c:v>0.192</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.192</c:v>
+                  <c:v>0.20979999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.20979999999999999</c:v>
+                  <c:v>0.25159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.25159999999999999</c:v>
+                  <c:v>0.27629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.27629999999999999</c:v>
+                  <c:v>0.3105</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.31040000000000001</c:v>
+                  <c:v>0.28270000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2659,7 +2697,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-A824-452F-B3EB-18D604DA1429}"/>
+              <c16:uniqueId val="{0000000E-D666-4F12-8625-2D8EC0377C1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3424,27 +3462,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>687458</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>57978</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>694594</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>32971</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>26186</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>13093</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A07836F-E5EF-4583-BF6B-86DDA818AE3E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7849C3A6-B43F-4E1E-9D5B-9F33EA78285F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3460,23 +3500,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Gerade Verbindung mit Pfeil 3">
+        <xdr:cNvPr id="3" name="Gerade Verbindung mit Pfeil 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA715ED9-0C6C-424F-9576-346538F5A989}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D745C8F-16E7-49BF-B6DF-78CAE4C9611D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3814,10 +3854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50CEFAE-1AD4-44A1-9917-42DDA6C5C118}">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3827,55 +3867,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>43890</v>
+        <v>43891</v>
       </c>
       <c r="C1" s="1">
-        <v>43891</v>
+        <v>43892</v>
       </c>
       <c r="D1" s="1">
-        <v>43892</v>
+        <v>43893</v>
       </c>
       <c r="E1" s="1">
-        <v>43893</v>
+        <v>43894</v>
       </c>
       <c r="F1" s="1">
-        <v>43894</v>
+        <v>43895</v>
       </c>
       <c r="G1" s="1">
-        <v>43895</v>
+        <v>43896</v>
       </c>
       <c r="H1" s="1">
-        <v>43896</v>
+        <v>43897</v>
       </c>
       <c r="I1" s="1">
-        <v>43897</v>
+        <v>43898</v>
       </c>
       <c r="J1" s="1">
-        <v>43898</v>
+        <v>43899</v>
       </c>
       <c r="K1" s="1">
-        <v>43899</v>
+        <v>43900</v>
       </c>
       <c r="L1" s="1">
-        <v>43900</v>
+        <v>43901</v>
       </c>
       <c r="M1" s="1">
-        <v>43901</v>
+        <v>43902</v>
       </c>
       <c r="N1" s="1">
-        <v>43902</v>
+        <v>43903</v>
       </c>
       <c r="O1" s="1">
-        <v>43903</v>
+        <v>43904</v>
       </c>
       <c r="P1" s="1">
-        <v>43904</v>
+        <v>43905</v>
       </c>
       <c r="Q1" s="1">
-        <v>43905</v>
+        <v>43906</v>
       </c>
       <c r="R1" s="1">
-        <v>43906</v>
+        <v>43907</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -3883,55 +3923,55 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>0.65490000000000004</v>
+        <v>0.59670000000000001</v>
       </c>
       <c r="C2" s="2">
-        <v>0.59670000000000001</v>
+        <v>0.55569999999999997</v>
       </c>
       <c r="D2" s="2">
-        <v>0.55569999999999997</v>
+        <v>0.60429999999999995</v>
       </c>
       <c r="E2" s="2">
-        <v>0.60429999999999995</v>
+        <v>0.4592</v>
       </c>
       <c r="F2" s="2">
-        <v>0.4592</v>
+        <v>0.36780000000000002</v>
       </c>
       <c r="G2" s="2">
+        <v>0.32140000000000002</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="I2" s="2">
         <v>0.36780000000000002</v>
       </c>
-      <c r="H2" s="2">
-        <v>0.32140000000000002</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.34799999999999998</v>
-      </c>
       <c r="J2" s="2">
-        <v>0.36780000000000002</v>
+        <v>0.3629</v>
       </c>
       <c r="K2" s="2">
-        <v>0.3629</v>
+        <v>0.35149999999999998</v>
       </c>
       <c r="L2" s="2">
-        <v>0.35149999999999998</v>
+        <v>0.33689999999999998</v>
       </c>
       <c r="M2" s="2">
-        <v>0.33689999999999998</v>
+        <v>0.32340000000000002</v>
       </c>
       <c r="N2" s="2">
-        <v>0.32340000000000002</v>
+        <v>0.35289999999999999</v>
       </c>
       <c r="O2" s="2">
-        <v>0.35289999999999999</v>
+        <v>0.36809999999999998</v>
       </c>
       <c r="P2" s="2">
-        <v>0.36809999999999998</v>
+        <v>0.37859999999999999</v>
       </c>
       <c r="Q2" s="2">
-        <v>0.37859999999999999</v>
+        <v>0.36480000000000001</v>
       </c>
       <c r="R2" s="2">
-        <v>0.36480000000000001</v>
+        <v>0.32169999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -3939,55 +3979,55 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>7.46E-2</v>
       </c>
       <c r="C3" s="2">
-        <v>7.46E-2</v>
+        <v>0.38379999999999997</v>
       </c>
       <c r="D3" s="2">
-        <v>0.38379999999999997</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="E3" s="2">
-        <v>0.66400000000000003</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="F3" s="2">
-        <v>0.95699999999999996</v>
+        <v>1.1533</v>
       </c>
       <c r="G3" s="2">
-        <v>1.1533</v>
+        <v>1.0167999999999999</v>
       </c>
       <c r="H3" s="2">
-        <v>1.0167999999999999</v>
+        <v>0.94330000000000003</v>
       </c>
       <c r="I3" s="2">
-        <v>0.94330000000000003</v>
+        <v>0.8155</v>
       </c>
       <c r="J3" s="2">
-        <v>0.8155</v>
+        <v>0.63060000000000005</v>
       </c>
       <c r="K3" s="2">
-        <v>0.63060000000000005</v>
+        <v>0.40339999999999998</v>
       </c>
       <c r="L3" s="2">
-        <v>0.40339999999999998</v>
+        <v>0.25740000000000002</v>
       </c>
       <c r="M3" s="2">
-        <v>0.25740000000000002</v>
+        <v>0.16980000000000001</v>
       </c>
       <c r="N3" s="2">
-        <v>0.16980000000000001</v>
+        <v>0.18210000000000001</v>
       </c>
       <c r="O3" s="2">
-        <v>0.18210000000000001</v>
+        <v>0.21959999999999999</v>
       </c>
       <c r="P3" s="2">
-        <v>0.21959999999999999</v>
+        <v>0.27010000000000001</v>
       </c>
       <c r="Q3" s="2">
-        <v>0.27010000000000001</v>
+        <v>0.30969999999999998</v>
       </c>
       <c r="R3" s="2">
-        <v>0.30969999999999998</v>
+        <v>0.28010000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -3995,55 +4035,55 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>0.1188</v>
+        <v>0.1603</v>
       </c>
       <c r="C4" s="2">
-        <v>0.1603</v>
+        <v>0.19339999999999999</v>
       </c>
       <c r="D4" s="2">
-        <v>0.19339999999999999</v>
+        <v>0.20830000000000001</v>
       </c>
       <c r="E4" s="2">
-        <v>0.20830000000000001</v>
+        <v>0.17630000000000001</v>
       </c>
       <c r="F4" s="2">
-        <v>0.17630000000000001</v>
+        <v>0.1459</v>
       </c>
       <c r="G4" s="2">
-        <v>0.1459</v>
+        <v>0.13780000000000001</v>
       </c>
       <c r="H4" s="2">
-        <v>0.13780000000000001</v>
+        <v>0.14660000000000001</v>
       </c>
       <c r="I4" s="2">
-        <v>0.14660000000000001</v>
+        <v>0.1671</v>
       </c>
       <c r="J4" s="2">
-        <v>0.1671</v>
+        <v>0.1817</v>
       </c>
       <c r="K4" s="2">
-        <v>0.1817</v>
+        <v>0.1661</v>
       </c>
       <c r="L4" s="2">
-        <v>0.1661</v>
+        <v>0.17180000000000001</v>
       </c>
       <c r="M4" s="2">
-        <v>0.17180000000000001</v>
+        <v>0.16159999999999999</v>
       </c>
       <c r="N4" s="2">
-        <v>0.16159999999999999</v>
+        <v>0.20860000000000001</v>
       </c>
       <c r="O4" s="2">
-        <v>0.20860000000000001</v>
+        <v>0.2303</v>
       </c>
       <c r="P4" s="2">
-        <v>0.2303</v>
+        <v>0.24629999999999999</v>
       </c>
       <c r="Q4" s="2">
-        <v>0.24629999999999999</v>
+        <v>0.29649999999999999</v>
       </c>
       <c r="R4" s="2">
-        <v>0.29649999999999999</v>
+        <v>0.28460000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -4051,46 +4091,46 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="C5" s="2">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="C5" s="2">
-        <v>5.4000000000000003E-3</v>
-      </c>
       <c r="D5" s="2">
-        <v>5.1999999999999998E-3</v>
+        <v>4.8999999999999998E-3</v>
       </c>
       <c r="E5" s="2">
-        <v>4.8999999999999998E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="F5" s="2">
-        <v>4.1000000000000003E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="G5" s="2">
-        <v>3.0999999999999999E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="H5" s="2">
-        <v>2.3E-3</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="I5" s="2">
-        <v>1.6999999999999999E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="J5" s="2">
-        <v>1.6000000000000001E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="K5" s="2">
-        <v>1.2999999999999999E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="L5" s="2">
-        <v>1E-3</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="M5" s="2">
-        <v>6.9999999999999999E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="N5" s="2">
-        <v>5.0000000000000001E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="O5" s="2">
-        <v>4.0000000000000002E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="P5" s="2">
         <v>2.9999999999999997E-4</v>
@@ -4107,55 +4147,55 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>0.50509999999999999</v>
+        <v>0.59809999999999997</v>
       </c>
       <c r="C6" s="2">
-        <v>0.59809999999999997</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="D6" s="2">
-        <v>0.56599999999999995</v>
+        <v>0.46810000000000002</v>
       </c>
       <c r="E6" s="2">
-        <v>0.46810000000000002</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="F6" s="2">
-        <v>0.36799999999999999</v>
+        <v>0.32029999999999997</v>
       </c>
       <c r="G6" s="2">
-        <v>0.32029999999999997</v>
+        <v>0.33169999999999999</v>
       </c>
       <c r="H6" s="2">
-        <v>0.33169999999999999</v>
+        <v>0.39579999999999999</v>
       </c>
       <c r="I6" s="2">
-        <v>0.39579999999999999</v>
+        <v>0.41620000000000001</v>
       </c>
       <c r="J6" s="2">
-        <v>0.41620000000000001</v>
+        <v>0.39560000000000001</v>
       </c>
       <c r="K6" s="2">
-        <v>0.39560000000000001</v>
+        <v>0.33</v>
       </c>
       <c r="L6" s="2">
-        <v>0.33</v>
+        <v>0.27689999999999998</v>
       </c>
       <c r="M6" s="2">
-        <v>0.27689999999999998</v>
+        <v>0.2341</v>
       </c>
       <c r="N6" s="2">
-        <v>0.23400000000000001</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="O6" s="2">
-        <v>0.25669999999999998</v>
+        <v>0.26040000000000002</v>
       </c>
       <c r="P6" s="2">
-        <v>0.26</v>
+        <v>0.24390000000000001</v>
       </c>
       <c r="Q6" s="2">
-        <v>0.24340000000000001</v>
+        <v>0.25240000000000001</v>
       </c>
       <c r="R6" s="2">
-        <v>0.25180000000000002</v>
+        <v>0.2298</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -4163,55 +4203,55 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0.37080000000000002</v>
+        <v>0.43859999999999999</v>
       </c>
       <c r="C7" s="2">
-        <v>0.43859999999999999</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="D7" s="2">
-        <v>0.42199999999999999</v>
+        <v>0.41489999999999999</v>
       </c>
       <c r="E7" s="2">
-        <v>0.41489999999999999</v>
+        <v>0.37419999999999998</v>
       </c>
       <c r="F7" s="2">
-        <v>0.37419999999999998</v>
+        <v>0.38290000000000002</v>
       </c>
       <c r="G7" s="2">
-        <v>0.38290000000000002</v>
+        <v>0.40010000000000001</v>
       </c>
       <c r="H7" s="2">
-        <v>0.40010000000000001</v>
+        <v>0.41620000000000001</v>
       </c>
       <c r="I7" s="2">
-        <v>0.41620000000000001</v>
+        <v>0.42009999999999997</v>
       </c>
       <c r="J7" s="2">
-        <v>0.42009999999999997</v>
+        <v>0.33829999999999999</v>
       </c>
       <c r="K7" s="2">
-        <v>0.33829999999999999</v>
+        <v>0.26950000000000002</v>
       </c>
       <c r="L7" s="2">
-        <v>0.26950000000000002</v>
+        <v>0.23519999999999999</v>
       </c>
       <c r="M7" s="2">
-        <v>0.23519999999999999</v>
+        <v>0.21360000000000001</v>
       </c>
       <c r="N7" s="2">
-        <v>0.21360000000000001</v>
+        <v>0.2626</v>
       </c>
       <c r="O7" s="2">
-        <v>0.2626</v>
+        <v>0.29530000000000001</v>
       </c>
       <c r="P7" s="2">
-        <v>0.29530000000000001</v>
+        <v>0.32640000000000002</v>
       </c>
       <c r="Q7" s="2">
-        <v>0.32640000000000002</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="R7" s="2">
-        <v>0.34200000000000003</v>
+        <v>0.30649999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -4222,52 +4262,52 @@
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>5.1400000000000001E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>5.1400000000000001E-2</v>
+        <v>9.6299999999999997E-2</v>
       </c>
       <c r="E8" s="2">
-        <v>9.6299999999999997E-2</v>
+        <v>0.4335</v>
       </c>
       <c r="F8" s="2">
-        <v>0.4335</v>
+        <v>0.62660000000000005</v>
       </c>
       <c r="G8" s="2">
-        <v>0.62660000000000005</v>
+        <v>0.68659999999999999</v>
       </c>
       <c r="H8" s="2">
-        <v>0.68659999999999999</v>
+        <v>0.64419999999999999</v>
       </c>
       <c r="I8" s="2">
-        <v>0.64419999999999999</v>
+        <v>0.28620000000000001</v>
       </c>
       <c r="J8" s="2">
-        <v>0.28620000000000001</v>
+        <v>0.16489999999999999</v>
       </c>
       <c r="K8" s="2">
-        <v>0.16489999999999999</v>
+        <v>0.1159</v>
       </c>
       <c r="L8" s="2">
-        <v>0.1159</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="M8" s="2">
-        <v>0.14099999999999999</v>
+        <v>0.1641</v>
       </c>
       <c r="N8" s="2">
-        <v>0.1641</v>
+        <v>0.16950000000000001</v>
       </c>
       <c r="O8" s="2">
-        <v>0.16950000000000001</v>
+        <v>0.16819999999999999</v>
       </c>
       <c r="P8" s="2">
-        <v>0.16819999999999999</v>
+        <v>0.16539999999999999</v>
       </c>
       <c r="Q8" s="2">
-        <v>0.16539999999999999</v>
+        <v>0.14990000000000001</v>
       </c>
       <c r="R8" s="2">
-        <v>0.14990000000000001</v>
+        <v>0.14580000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -4275,55 +4315,55 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.57550000000000001</v>
+        <v>0.60529999999999995</v>
       </c>
       <c r="C9" s="2">
-        <v>0.60529999999999995</v>
+        <v>0.59140000000000004</v>
       </c>
       <c r="D9" s="2">
-        <v>0.59140000000000004</v>
+        <v>0.58030000000000004</v>
       </c>
       <c r="E9" s="2">
-        <v>0.58030000000000004</v>
+        <v>0.5323</v>
       </c>
       <c r="F9" s="2">
-        <v>0.5323</v>
+        <v>0.4546</v>
       </c>
       <c r="G9" s="2">
-        <v>0.4546</v>
+        <v>0.38129999999999997</v>
       </c>
       <c r="H9" s="2">
-        <v>0.38129999999999997</v>
+        <v>0.30769999999999997</v>
       </c>
       <c r="I9" s="2">
-        <v>0.30769999999999997</v>
+        <v>0.26179999999999998</v>
       </c>
       <c r="J9" s="2">
-        <v>0.26179999999999998</v>
+        <v>0.22189999999999999</v>
       </c>
       <c r="K9" s="2">
-        <v>0.22189999999999999</v>
+        <v>0.1812</v>
       </c>
       <c r="L9" s="2">
-        <v>0.1812</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="M9" s="2">
-        <v>0.14499999999999999</v>
+        <v>0.1216</v>
       </c>
       <c r="N9" s="2">
-        <v>0.1216</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="O9" s="2">
-        <v>0.11700000000000001</v>
+        <v>0.1193</v>
       </c>
       <c r="P9" s="2">
-        <v>0.1193</v>
+        <v>0.1196</v>
       </c>
       <c r="Q9" s="2">
-        <v>0.1196</v>
+        <v>0.1133</v>
       </c>
       <c r="R9" s="2">
-        <v>0.1133</v>
+        <v>0.1033</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -4331,55 +4371,55 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.3947</v>
+        <v>0.38650000000000001</v>
       </c>
       <c r="C10" s="2">
-        <v>0.38650000000000001</v>
+        <v>0.35759999999999997</v>
       </c>
       <c r="D10" s="2">
-        <v>0.35759999999999997</v>
+        <v>0.32929999999999998</v>
       </c>
       <c r="E10" s="2">
-        <v>0.32929999999999998</v>
+        <v>0.2999</v>
       </c>
       <c r="F10" s="2">
-        <v>0.2999</v>
+        <v>0.26329999999999998</v>
       </c>
       <c r="G10" s="2">
-        <v>0.26329999999999998</v>
+        <v>0.24260000000000001</v>
       </c>
       <c r="H10" s="2">
-        <v>0.24260000000000001</v>
+        <v>0.2324</v>
       </c>
       <c r="I10" s="2">
-        <v>0.2324</v>
+        <v>0.23760000000000001</v>
       </c>
       <c r="J10" s="2">
-        <v>0.23760000000000001</v>
+        <v>0.24129999999999999</v>
       </c>
       <c r="K10" s="2">
-        <v>0.24129999999999999</v>
+        <v>0.2321</v>
       </c>
       <c r="L10" s="2">
-        <v>0.2321</v>
+        <v>0.21940000000000001</v>
       </c>
       <c r="M10" s="2">
-        <v>0.21940000000000001</v>
+        <v>0.1832</v>
       </c>
       <c r="N10" s="2">
-        <v>0.1832</v>
+        <v>0.17380000000000001</v>
       </c>
       <c r="O10" s="2">
-        <v>0.17380000000000001</v>
+        <v>0.17730000000000001</v>
       </c>
       <c r="P10" s="2">
-        <v>0.17730000000000001</v>
+        <v>0.18920000000000001</v>
       </c>
       <c r="Q10" s="2">
-        <v>0.18920000000000001</v>
+        <v>0.20469999999999999</v>
       </c>
       <c r="R10" s="2">
-        <v>0.20469999999999999</v>
+        <v>0.18590000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -4387,55 +4427,55 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.31680000000000003</v>
+        <v>0.31640000000000001</v>
       </c>
       <c r="C11" s="2">
-        <v>0.31640000000000001</v>
+        <v>0.29389999999999999</v>
       </c>
       <c r="D11" s="2">
-        <v>0.29389999999999999</v>
+        <v>0.25380000000000003</v>
       </c>
       <c r="E11" s="2">
-        <v>0.25380000000000003</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="F11" s="2">
-        <v>0.20200000000000001</v>
+        <v>0.16339999999999999</v>
       </c>
       <c r="G11" s="2">
-        <v>0.16339999999999999</v>
+        <v>0.13009999999999999</v>
       </c>
       <c r="H11" s="2">
-        <v>0.13009999999999999</v>
+        <v>0.10440000000000001</v>
       </c>
       <c r="I11" s="2">
-        <v>0.10440000000000001</v>
+        <v>8.4500000000000006E-2</v>
       </c>
       <c r="J11" s="2">
-        <v>8.4500000000000006E-2</v>
+        <v>6.6199999999999995E-2</v>
       </c>
       <c r="K11" s="2">
-        <v>6.6199999999999995E-2</v>
+        <v>5.0700000000000002E-2</v>
       </c>
       <c r="L11" s="2">
-        <v>5.0700000000000002E-2</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="M11" s="2">
-        <v>3.6299999999999999E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="N11" s="2">
-        <v>2.52E-2</v>
+        <v>1.9699999999999999E-2</v>
       </c>
       <c r="O11" s="2">
-        <v>1.9699999999999999E-2</v>
+        <v>1.78E-2</v>
       </c>
       <c r="P11" s="2">
-        <v>1.78E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="Q11" s="2">
-        <v>1.5900000000000001E-2</v>
+        <v>1.4200000000000001E-2</v>
       </c>
       <c r="R11" s="2">
-        <v>1.4200000000000001E-2</v>
+        <v>1.1599999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -4443,55 +4483,55 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.74160000000000004</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="C12" s="2">
-        <v>0.66400000000000003</v>
+        <v>0.64510000000000001</v>
       </c>
       <c r="D12" s="2">
-        <v>0.64510000000000001</v>
+        <v>0.57479999999999998</v>
       </c>
       <c r="E12" s="2">
-        <v>0.57479999999999998</v>
+        <v>0.53220000000000001</v>
       </c>
       <c r="F12" s="2">
-        <v>0.53220000000000001</v>
+        <v>0.4153</v>
       </c>
       <c r="G12" s="2">
-        <v>0.4153</v>
+        <v>0.3715</v>
       </c>
       <c r="H12" s="2">
-        <v>0.3715</v>
+        <v>0.33129999999999998</v>
       </c>
       <c r="I12" s="2">
-        <v>0.33129999999999998</v>
+        <v>0.32719999999999999</v>
       </c>
       <c r="J12" s="2">
-        <v>0.32719999999999999</v>
+        <v>0.36549999999999999</v>
       </c>
       <c r="K12" s="2">
-        <v>0.36549999999999999</v>
+        <v>0.40579999999999999</v>
       </c>
       <c r="L12" s="2">
-        <v>0.40579999999999999</v>
+        <v>0.44440000000000002</v>
       </c>
       <c r="M12" s="2">
-        <v>0.44440000000000002</v>
+        <v>0.4118</v>
       </c>
       <c r="N12" s="2">
-        <v>0.4118</v>
+        <v>0.44479999999999997</v>
       </c>
       <c r="O12" s="2">
-        <v>0.44479999999999997</v>
+        <v>0.41770000000000002</v>
       </c>
       <c r="P12" s="2">
-        <v>0.41770000000000002</v>
+        <v>0.4007</v>
       </c>
       <c r="Q12" s="2">
-        <v>0.4007</v>
+        <v>0.40179999999999999</v>
       </c>
       <c r="R12" s="2">
-        <v>0.40179999999999999</v>
+        <v>0.3175</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -4499,55 +4539,55 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.71579999999999999</v>
+        <v>0.69479999999999997</v>
       </c>
       <c r="C13" s="2">
-        <v>0.69479999999999997</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="D13" s="2">
-        <v>0.42299999999999999</v>
+        <v>0.3296</v>
       </c>
       <c r="E13" s="2">
-        <v>0.3296</v>
+        <v>0.28549999999999998</v>
       </c>
       <c r="F13" s="2">
-        <v>0.28549999999999998</v>
+        <v>0.46010000000000001</v>
       </c>
       <c r="G13" s="2">
-        <v>0.46010000000000001</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="H13" s="2">
-        <v>0.53900000000000003</v>
+        <v>0.63349999999999995</v>
       </c>
       <c r="I13" s="2">
-        <v>0.63349999999999995</v>
+        <v>0.59970000000000001</v>
       </c>
       <c r="J13" s="2">
-        <v>0.59970000000000001</v>
+        <v>0.42120000000000002</v>
       </c>
       <c r="K13" s="2">
-        <v>0.42120000000000002</v>
+        <v>0.36820000000000003</v>
       </c>
       <c r="L13" s="2">
-        <v>0.36820000000000003</v>
+        <v>0.32669999999999999</v>
       </c>
       <c r="M13" s="2">
-        <v>0.32669999999999999</v>
+        <v>0.32979999999999998</v>
       </c>
       <c r="N13" s="2">
-        <v>0.32979999999999998</v>
+        <v>0.32969999999999999</v>
       </c>
       <c r="O13" s="2">
-        <v>0.32969999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="P13" s="2">
-        <v>0.31</v>
+        <v>0.26190000000000002</v>
       </c>
       <c r="Q13" s="2">
-        <v>0.26190000000000002</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="R13" s="2">
-        <v>0.20699999999999999</v>
+        <v>0.14729999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -4555,55 +4595,55 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>1.4147000000000001</v>
+        <v>1.2688999999999999</v>
       </c>
       <c r="C14" s="2">
-        <v>1.2688999999999999</v>
+        <v>0.71740000000000004</v>
       </c>
       <c r="D14" s="2">
-        <v>0.71740000000000004</v>
+        <v>0.64670000000000005</v>
       </c>
       <c r="E14" s="2">
-        <v>0.64670000000000005</v>
+        <v>0.53349999999999997</v>
       </c>
       <c r="F14" s="2">
-        <v>0.53349999999999997</v>
+        <v>0.48820000000000002</v>
       </c>
       <c r="G14" s="2">
-        <v>0.48820000000000002</v>
+        <v>0.48049999999999998</v>
       </c>
       <c r="H14" s="2">
-        <v>0.48049999999999998</v>
+        <v>0.47770000000000001</v>
       </c>
       <c r="I14" s="2">
-        <v>0.47770000000000001</v>
+        <v>0.44469999999999998</v>
       </c>
       <c r="J14" s="2">
-        <v>0.44469999999999998</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="K14" s="2">
-        <v>0.39300000000000002</v>
+        <v>0.30220000000000002</v>
       </c>
       <c r="L14" s="2">
-        <v>0.30220000000000002</v>
+        <v>0.2631</v>
       </c>
       <c r="M14" s="2">
-        <v>0.2631</v>
+        <v>0.2167</v>
       </c>
       <c r="N14" s="2">
-        <v>0.2167</v>
+        <v>0.25690000000000002</v>
       </c>
       <c r="O14" s="2">
-        <v>0.25690000000000002</v>
+        <v>0.27229999999999999</v>
       </c>
       <c r="P14" s="2">
-        <v>0.27229999999999999</v>
+        <v>0.3266</v>
       </c>
       <c r="Q14" s="2">
-        <v>0.3266</v>
+        <v>0.33839999999999998</v>
       </c>
       <c r="R14" s="2">
-        <v>0.33839999999999998</v>
+        <v>0.30570000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -4649,17 +4689,17 @@
       <c r="N15" t="s">
         <v>15</v>
       </c>
-      <c r="O15" t="s">
-        <v>15</v>
+      <c r="O15">
+        <v>0.63460000000000005</v>
       </c>
       <c r="P15" s="2">
-        <v>0.63460000000000005</v>
+        <v>0.40489999999999998</v>
       </c>
       <c r="Q15" s="2">
-        <v>0.40489999999999998</v>
+        <v>0.30259999999999998</v>
       </c>
       <c r="R15" s="2">
-        <v>0.30259999999999998</v>
+        <v>0.30669999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -4667,141 +4707,215 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1346</v>
+        <v>0.193</v>
       </c>
       <c r="C16" s="2">
-        <v>0.193</v>
+        <v>0.24660000000000001</v>
       </c>
       <c r="D16" s="2">
-        <v>0.24660000000000001</v>
+        <v>0.27539999999999998</v>
       </c>
       <c r="E16" s="2">
-        <v>0.27539999999999998</v>
+        <v>0.32169999999999999</v>
       </c>
       <c r="F16" s="2">
-        <v>0.32169999999999999</v>
+        <v>0.3377</v>
       </c>
       <c r="G16" s="2">
-        <v>0.3377</v>
-      </c>
-      <c r="H16" s="2"/>
+        <v>0.3866</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.39939999999999998</v>
+      </c>
       <c r="I16" s="2">
-        <v>0.39939999999999998</v>
+        <v>0.38159999999999999</v>
       </c>
       <c r="J16" s="2">
-        <v>0.38159999999999999</v>
+        <v>0.3347</v>
       </c>
       <c r="K16" s="2">
-        <v>0.3347</v>
+        <v>0.2792</v>
       </c>
       <c r="L16" s="2">
-        <v>0.2792</v>
+        <v>0.2437</v>
       </c>
       <c r="M16" s="2">
-        <v>0.2437</v>
+        <v>0.192</v>
       </c>
       <c r="N16" s="2">
-        <v>0.192</v>
+        <v>0.20979999999999999</v>
       </c>
       <c r="O16" s="2">
-        <v>0.20979999999999999</v>
+        <v>0.25159999999999999</v>
       </c>
       <c r="P16" s="2">
-        <v>0.25159999999999999</v>
+        <v>0.27629999999999999</v>
       </c>
       <c r="Q16" s="2">
-        <v>0.27629999999999999</v>
+        <v>0.3105</v>
       </c>
       <c r="R16" s="2">
-        <v>0.31040000000000001</v>
+        <v>0.28270000000000001</v>
       </c>
     </row>
-    <row r="34" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E356A6A6-24A0-42A0-8188-ED9E5DA792BF}">
+  <dimension ref="B33:M48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="L36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
+      </c>
+      <c r="L37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="L38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D44" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G34" t="s">
+      <c r="E44" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="J44" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" t="s">
-        <v>21</v>
-      </c>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D45" s="4"/>
+      <c r="E45" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J45" s="6"/>
     </row>
-    <row r="36" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" t="s">
-        <v>19</v>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G47" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="37" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E37" s="3">
-        <v>0</v>
-      </c>
-      <c r="G37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
         <v>26</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J40" t="s">
-        <v>30</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L40" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="G41" s="4"/>
-      <c r="H41" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I41" s="6"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M41" s="6"/>
-    </row>
-    <row r="43" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="J43" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="J44" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2020-03-19 06:50 New data
</commit_message>
<xml_diff>
--- a/COVID-19 Apps/Growth Chart.xlsx
+++ b/COVID-19 Apps/Growth Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zur Bonsen Georg\Documents\Programme\Beyond4P_Apps\COVID-19 Apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A33A65-A1A6-48FA-881C-6565E1EBEF51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE760A5-2077-4027-B8BD-B87D4B18EF8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{A4C1FE6B-DE9B-48BC-897C-015B097916DC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Country/Region</t>
   </si>
@@ -420,55 +420,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -480,55 +480,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.59670000000000001</c:v>
+                  <c:v>0.55569999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55569999999999997</c:v>
+                  <c:v>0.60429999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60429999999999995</c:v>
+                  <c:v>0.4592</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4592</c:v>
+                  <c:v>0.36780000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.32140000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.36780000000000002</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32140000000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.34799999999999998</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.36780000000000002</c:v>
+                  <c:v>0.3629</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3629</c:v>
+                  <c:v>0.35149999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.35149999999999998</c:v>
+                  <c:v>0.33689999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33689999999999998</c:v>
+                  <c:v>0.32340000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32340000000000002</c:v>
+                  <c:v>0.35289999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.35289999999999999</c:v>
+                  <c:v>0.36809999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.36809999999999998</c:v>
+                  <c:v>0.37859999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.37859999999999999</c:v>
+                  <c:v>0.36480000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.36480000000000001</c:v>
+                  <c:v>0.32169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32169999999999999</c:v>
+                  <c:v>0.28599999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,55 +573,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,55 +633,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>7.46E-2</c:v>
+                  <c:v>0.38379999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38379999999999997</c:v>
+                  <c:v>0.66400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66400000000000003</c:v>
+                  <c:v>0.95699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95699999999999996</c:v>
+                  <c:v>1.1533</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1533</c:v>
+                  <c:v>1.0167999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0167999999999999</c:v>
+                  <c:v>0.94330000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.94330000000000003</c:v>
+                  <c:v>0.8155</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8155</c:v>
+                  <c:v>0.63060000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.63060000000000005</c:v>
+                  <c:v>0.40339999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.40339999999999998</c:v>
+                  <c:v>0.25740000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25740000000000002</c:v>
+                  <c:v>0.16980000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16980000000000001</c:v>
+                  <c:v>0.18210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.18210000000000001</c:v>
+                  <c:v>0.21959999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.21959999999999999</c:v>
+                  <c:v>0.27010000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.27010000000000001</c:v>
+                  <c:v>0.30969999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.30969999999999998</c:v>
+                  <c:v>0.28010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28010000000000002</c:v>
+                  <c:v>0.24779999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,55 +726,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -786,55 +786,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.1603</c:v>
+                  <c:v>0.19339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19339999999999999</c:v>
+                  <c:v>0.20830000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20830000000000001</c:v>
+                  <c:v>0.17630000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17630000000000001</c:v>
+                  <c:v>0.1459</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1459</c:v>
+                  <c:v>0.13780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13780000000000001</c:v>
+                  <c:v>0.14660000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14660000000000001</c:v>
+                  <c:v>0.1671</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1671</c:v>
+                  <c:v>0.1817</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1817</c:v>
+                  <c:v>0.1661</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1661</c:v>
+                  <c:v>0.17180000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.17180000000000001</c:v>
+                  <c:v>0.16159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16159999999999999</c:v>
+                  <c:v>0.20860000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.20860000000000001</c:v>
+                  <c:v>0.2303</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2303</c:v>
+                  <c:v>0.24629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.24629999999999999</c:v>
+                  <c:v>0.29649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.29649999999999999</c:v>
+                  <c:v>0.28460000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28460000000000002</c:v>
+                  <c:v>0.32019999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -879,55 +879,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -939,43 +939,43 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>5.4000000000000003E-3</c:v>
+                  <c:v>5.1999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1999999999999998E-3</c:v>
+                  <c:v>4.8999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8999999999999998E-3</c:v>
+                  <c:v>4.1000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1000000000000003E-3</c:v>
+                  <c:v>3.0999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0999999999999999E-3</c:v>
+                  <c:v>2.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3E-3</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6999999999999999E-3</c:v>
+                  <c:v>1.6000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6000000000000001E-3</c:v>
+                  <c:v>1.2999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2999999999999999E-3</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1E-3</c:v>
+                  <c:v>6.9999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.9999999999999999E-4</c:v>
+                  <c:v>5.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.0000000000000001E-4</c:v>
+                  <c:v>4.0000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0000000000000002E-4</c:v>
+                  <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2.9999999999999997E-4</c:v>
@@ -1033,55 +1033,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1093,55 +1093,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.59809999999999997</c:v>
+                  <c:v>0.56599999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56599999999999995</c:v>
+                  <c:v>0.46810000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46810000000000002</c:v>
+                  <c:v>0.36799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36799999999999999</c:v>
+                  <c:v>0.32029999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32029999999999997</c:v>
+                  <c:v>0.33169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.33169999999999999</c:v>
+                  <c:v>0.39579999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39579999999999999</c:v>
+                  <c:v>0.41620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.41620000000000001</c:v>
+                  <c:v>0.39560000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39560000000000001</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33</c:v>
+                  <c:v>0.27689999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.27689999999999998</c:v>
+                  <c:v>0.2341</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2341</c:v>
+                  <c:v>0.25700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25700000000000001</c:v>
+                  <c:v>0.26040000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26040000000000002</c:v>
+                  <c:v>0.24390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.24390000000000001</c:v>
+                  <c:v>0.25240000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.25240000000000001</c:v>
+                  <c:v>0.2298</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.2298</c:v>
+                  <c:v>0.22409999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1186,55 +1186,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,55 +1246,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.43859999999999999</c:v>
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42199999999999999</c:v>
+                  <c:v>0.41489999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41489999999999999</c:v>
+                  <c:v>0.37419999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.37419999999999998</c:v>
+                  <c:v>0.38290000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38290000000000002</c:v>
+                  <c:v>0.40010000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.40010000000000001</c:v>
+                  <c:v>0.41620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.41620000000000001</c:v>
+                  <c:v>0.42009999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.42009999999999997</c:v>
+                  <c:v>0.33829999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33829999999999999</c:v>
+                  <c:v>0.26950000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.26950000000000002</c:v>
+                  <c:v>0.23519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.23519999999999999</c:v>
+                  <c:v>0.21360000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.21360000000000001</c:v>
+                  <c:v>0.2626</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2626</c:v>
+                  <c:v>0.29530000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.29530000000000001</c:v>
+                  <c:v>0.32640000000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.32640000000000002</c:v>
+                  <c:v>0.34200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.34200000000000003</c:v>
+                  <c:v>0.30649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.30649999999999999</c:v>
+                  <c:v>0.29260000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1339,55 +1339,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1399,55 +1399,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.1400000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1400000000000001E-2</c:v>
+                  <c:v>9.6299999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6299999999999997E-2</c:v>
+                  <c:v>0.4335</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4335</c:v>
+                  <c:v>0.62660000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.62660000000000005</c:v>
+                  <c:v>0.68659999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68659999999999999</c:v>
+                  <c:v>0.64419999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.64419999999999999</c:v>
+                  <c:v>0.28620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.28620000000000001</c:v>
+                  <c:v>0.16489999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16489999999999999</c:v>
+                  <c:v>0.1159</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1159</c:v>
+                  <c:v>0.14099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14099999999999999</c:v>
+                  <c:v>0.1641</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1641</c:v>
+                  <c:v>0.16950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16950000000000001</c:v>
+                  <c:v>0.16819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.16819999999999999</c:v>
+                  <c:v>0.16539999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.16539999999999999</c:v>
+                  <c:v>0.14990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.14990000000000001</c:v>
+                  <c:v>0.14580000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.14580000000000001</c:v>
+                  <c:v>0.12859999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1494,55 +1494,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1554,55 +1554,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.60529999999999995</c:v>
+                  <c:v>0.59140000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59140000000000004</c:v>
+                  <c:v>0.58030000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58030000000000004</c:v>
+                  <c:v>0.5323</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5323</c:v>
+                  <c:v>0.4546</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4546</c:v>
+                  <c:v>0.38129999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38129999999999997</c:v>
+                  <c:v>0.30769999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.30769999999999997</c:v>
+                  <c:v>0.26179999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26179999999999998</c:v>
+                  <c:v>0.22189999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.22189999999999999</c:v>
+                  <c:v>0.1812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1812</c:v>
+                  <c:v>0.14499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14499999999999999</c:v>
+                  <c:v>0.1216</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1216</c:v>
+                  <c:v>0.11700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.11700000000000001</c:v>
+                  <c:v>0.1193</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1193</c:v>
+                  <c:v>0.1196</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1196</c:v>
+                  <c:v>0.1133</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1133</c:v>
+                  <c:v>0.1033</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1033</c:v>
+                  <c:v>9.1600000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1647,55 +1647,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1707,55 +1707,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.38650000000000001</c:v>
+                  <c:v>0.35759999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35759999999999997</c:v>
+                  <c:v>0.32929999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32929999999999998</c:v>
+                  <c:v>0.2999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2999</c:v>
+                  <c:v>0.26329999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.26329999999999998</c:v>
+                  <c:v>0.24260000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24260000000000001</c:v>
+                  <c:v>0.2324</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2324</c:v>
+                  <c:v>0.23760000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23760000000000001</c:v>
+                  <c:v>0.24129999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.24129999999999999</c:v>
+                  <c:v>0.2321</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2321</c:v>
+                  <c:v>0.21940000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.21940000000000001</c:v>
+                  <c:v>0.1832</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1832</c:v>
+                  <c:v>0.17380000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.17380000000000001</c:v>
+                  <c:v>0.17730000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.17730000000000001</c:v>
+                  <c:v>0.18920000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.18920000000000001</c:v>
+                  <c:v>0.20469999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.20469999999999999</c:v>
+                  <c:v>0.18590000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.18590000000000001</c:v>
+                  <c:v>0.1673</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1802,55 +1802,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1862,55 +1862,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.31640000000000001</c:v>
+                  <c:v>0.29389999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29389999999999999</c:v>
+                  <c:v>0.25380000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25380000000000003</c:v>
+                  <c:v>0.20200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20200000000000001</c:v>
+                  <c:v>0.16339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16339999999999999</c:v>
+                  <c:v>0.13009999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13009999999999999</c:v>
+                  <c:v>0.10440000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10440000000000001</c:v>
+                  <c:v>8.4500000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4500000000000006E-2</c:v>
+                  <c:v>6.6199999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.6199999999999995E-2</c:v>
+                  <c:v>5.0700000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.0700000000000002E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.6299999999999999E-2</c:v>
+                  <c:v>2.52E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.52E-2</c:v>
+                  <c:v>1.9699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9699999999999999E-2</c:v>
+                  <c:v>1.78E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.78E-2</c:v>
+                  <c:v>1.5900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5900000000000001E-2</c:v>
+                  <c:v>1.4200000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4200000000000001E-2</c:v>
+                  <c:v>1.1599999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1599999999999999E-2</c:v>
+                  <c:v>1.06E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1958,55 +1958,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2018,55 +2018,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.66400000000000003</c:v>
+                  <c:v>0.64510000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64510000000000001</c:v>
+                  <c:v>0.57479999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.57479999999999998</c:v>
+                  <c:v>0.53220000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53220000000000001</c:v>
+                  <c:v>0.4153</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4153</c:v>
+                  <c:v>0.3715</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3715</c:v>
+                  <c:v>0.33129999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.33129999999999998</c:v>
+                  <c:v>0.32719999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32719999999999999</c:v>
+                  <c:v>0.36549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36549999999999999</c:v>
+                  <c:v>0.40579999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.40579999999999999</c:v>
+                  <c:v>0.44440000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.44440000000000002</c:v>
+                  <c:v>0.4118</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4118</c:v>
+                  <c:v>0.44479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.44479999999999997</c:v>
+                  <c:v>0.41770000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.41770000000000002</c:v>
+                  <c:v>0.4007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.4007</c:v>
+                  <c:v>0.40179999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.40179999999999999</c:v>
+                  <c:v>0.3175</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.3175</c:v>
+                  <c:v>0.2651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2111,55 +2111,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2171,55 +2171,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.69479999999999997</c:v>
+                  <c:v>0.42299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42299999999999999</c:v>
+                  <c:v>0.3296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3296</c:v>
+                  <c:v>0.28549999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28549999999999998</c:v>
+                  <c:v>0.46010000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46010000000000001</c:v>
+                  <c:v>0.53900000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.53900000000000003</c:v>
+                  <c:v>0.63349999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.63349999999999995</c:v>
+                  <c:v>0.59970000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.59970000000000001</c:v>
+                  <c:v>0.42120000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.42120000000000002</c:v>
+                  <c:v>0.36820000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36820000000000003</c:v>
+                  <c:v>0.32669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.32669999999999999</c:v>
+                  <c:v>0.32979999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32979999999999998</c:v>
+                  <c:v>0.32969999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.32969999999999999</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.31</c:v>
+                  <c:v>0.26190000000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.26190000000000002</c:v>
+                  <c:v>0.20699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.20699999999999999</c:v>
+                  <c:v>0.14729999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.14729999999999999</c:v>
+                  <c:v>0.1075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2268,55 +2268,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,55 +2328,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.2688999999999999</c:v>
+                  <c:v>0.71740000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71740000000000004</c:v>
+                  <c:v>0.64670000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64670000000000005</c:v>
+                  <c:v>0.53349999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53349999999999997</c:v>
+                  <c:v>0.48820000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48820000000000002</c:v>
+                  <c:v>0.48049999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48049999999999998</c:v>
+                  <c:v>0.47770000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47770000000000001</c:v>
+                  <c:v>0.44469999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44469999999999998</c:v>
+                  <c:v>0.39300000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39300000000000002</c:v>
+                  <c:v>0.30220000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.30220000000000002</c:v>
+                  <c:v>0.2631</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2631</c:v>
+                  <c:v>0.2167</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2167</c:v>
+                  <c:v>0.25690000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25690000000000002</c:v>
+                  <c:v>0.27229999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27229999999999999</c:v>
+                  <c:v>0.3266</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.3266</c:v>
+                  <c:v>0.33839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.33839999999999998</c:v>
+                  <c:v>0.30570000000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.30570000000000003</c:v>
+                  <c:v>0.25950000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,55 +2425,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2520,20 +2520,20 @@
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="12" formatCode="0.00%">
                   <c:v>0.63460000000000005</c:v>
                 </c:pt>
+                <c:pt idx="13" formatCode="0.00%">
+                  <c:v>0.40489999999999998</c:v>
+                </c:pt>
                 <c:pt idx="14" formatCode="0.00%">
-                  <c:v>0.40489999999999998</c:v>
+                  <c:v>0.30259999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00%">
-                  <c:v>0.30259999999999998</c:v>
+                  <c:v>0.30669999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00%">
-                  <c:v>0.30669999999999997</c:v>
+                  <c:v>0.30790000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2581,55 +2581,55 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43891</c:v>
+                  <c:v>43892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43893</c:v>
+                  <c:v>43894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43894</c:v>
+                  <c:v>43895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43895</c:v>
+                  <c:v>43896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43896</c:v>
+                  <c:v>43897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43897</c:v>
+                  <c:v>43898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43898</c:v>
+                  <c:v>43899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43899</c:v>
+                  <c:v>43900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43900</c:v>
+                  <c:v>43901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43901</c:v>
+                  <c:v>43902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43902</c:v>
+                  <c:v>43903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43903</c:v>
+                  <c:v>43904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43904</c:v>
+                  <c:v>43905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43905</c:v>
+                  <c:v>43906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43906</c:v>
+                  <c:v>43907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43907</c:v>
+                  <c:v>43908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2641,55 +2641,55 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.193</c:v>
+                  <c:v>0.24660000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24660000000000001</c:v>
+                  <c:v>0.27539999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27539999999999998</c:v>
+                  <c:v>0.32169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32169999999999999</c:v>
+                  <c:v>0.3377</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3377</c:v>
+                  <c:v>0.3866</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3866</c:v>
+                  <c:v>0.39939999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39939999999999998</c:v>
+                  <c:v>0.38159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.38159999999999999</c:v>
+                  <c:v>0.3347</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3347</c:v>
+                  <c:v>0.2792</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2792</c:v>
+                  <c:v>0.2437</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2437</c:v>
+                  <c:v>0.192</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.192</c:v>
+                  <c:v>0.20979999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.20979999999999999</c:v>
+                  <c:v>0.25159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.25159999999999999</c:v>
+                  <c:v>0.27629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.27629999999999999</c:v>
+                  <c:v>0.3105</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.3105</c:v>
+                  <c:v>0.28270000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28270000000000001</c:v>
+                  <c:v>0.26469999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3856,8 +3856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50CEFAE-1AD4-44A1-9917-42DDA6C5C118}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:N45"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3867,55 +3867,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>43891</v>
+        <v>43892</v>
       </c>
       <c r="C1" s="1">
-        <v>43892</v>
+        <v>43893</v>
       </c>
       <c r="D1" s="1">
-        <v>43893</v>
+        <v>43894</v>
       </c>
       <c r="E1" s="1">
-        <v>43894</v>
+        <v>43895</v>
       </c>
       <c r="F1" s="1">
-        <v>43895</v>
+        <v>43896</v>
       </c>
       <c r="G1" s="1">
-        <v>43896</v>
+        <v>43897</v>
       </c>
       <c r="H1" s="1">
-        <v>43897</v>
+        <v>43898</v>
       </c>
       <c r="I1" s="1">
-        <v>43898</v>
+        <v>43899</v>
       </c>
       <c r="J1" s="1">
-        <v>43899</v>
+        <v>43900</v>
       </c>
       <c r="K1" s="1">
-        <v>43900</v>
+        <v>43901</v>
       </c>
       <c r="L1" s="1">
-        <v>43901</v>
+        <v>43902</v>
       </c>
       <c r="M1" s="1">
-        <v>43902</v>
+        <v>43903</v>
       </c>
       <c r="N1" s="1">
-        <v>43903</v>
+        <v>43904</v>
       </c>
       <c r="O1" s="1">
-        <v>43904</v>
+        <v>43905</v>
       </c>
       <c r="P1" s="1">
-        <v>43905</v>
+        <v>43906</v>
       </c>
       <c r="Q1" s="1">
-        <v>43906</v>
+        <v>43907</v>
       </c>
       <c r="R1" s="1">
-        <v>43907</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -3923,55 +3923,55 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>0.59670000000000001</v>
+        <v>0.55569999999999997</v>
       </c>
       <c r="C2" s="2">
-        <v>0.55569999999999997</v>
+        <v>0.60429999999999995</v>
       </c>
       <c r="D2" s="2">
-        <v>0.60429999999999995</v>
+        <v>0.4592</v>
       </c>
       <c r="E2" s="2">
-        <v>0.4592</v>
+        <v>0.36780000000000002</v>
       </c>
       <c r="F2" s="2">
+        <v>0.32140000000000002</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="H2" s="2">
         <v>0.36780000000000002</v>
       </c>
-      <c r="G2" s="2">
-        <v>0.32140000000000002</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.34799999999999998</v>
-      </c>
       <c r="I2" s="2">
-        <v>0.36780000000000002</v>
+        <v>0.3629</v>
       </c>
       <c r="J2" s="2">
-        <v>0.3629</v>
+        <v>0.35149999999999998</v>
       </c>
       <c r="K2" s="2">
-        <v>0.35149999999999998</v>
+        <v>0.33689999999999998</v>
       </c>
       <c r="L2" s="2">
-        <v>0.33689999999999998</v>
+        <v>0.32340000000000002</v>
       </c>
       <c r="M2" s="2">
-        <v>0.32340000000000002</v>
+        <v>0.35289999999999999</v>
       </c>
       <c r="N2" s="2">
-        <v>0.35289999999999999</v>
+        <v>0.36809999999999998</v>
       </c>
       <c r="O2" s="2">
-        <v>0.36809999999999998</v>
+        <v>0.37859999999999999</v>
       </c>
       <c r="P2" s="2">
-        <v>0.37859999999999999</v>
+        <v>0.36480000000000001</v>
       </c>
       <c r="Q2" s="2">
-        <v>0.36480000000000001</v>
+        <v>0.32169999999999999</v>
       </c>
       <c r="R2" s="2">
-        <v>0.32169999999999999</v>
+        <v>0.28599999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -3979,55 +3979,55 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>7.46E-2</v>
+        <v>0.38379999999999997</v>
       </c>
       <c r="C3" s="2">
-        <v>0.38379999999999997</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="D3" s="2">
-        <v>0.66400000000000003</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="E3" s="2">
-        <v>0.95699999999999996</v>
+        <v>1.1533</v>
       </c>
       <c r="F3" s="2">
-        <v>1.1533</v>
+        <v>1.0167999999999999</v>
       </c>
       <c r="G3" s="2">
-        <v>1.0167999999999999</v>
+        <v>0.94330000000000003</v>
       </c>
       <c r="H3" s="2">
-        <v>0.94330000000000003</v>
+        <v>0.8155</v>
       </c>
       <c r="I3" s="2">
-        <v>0.8155</v>
+        <v>0.63060000000000005</v>
       </c>
       <c r="J3" s="2">
-        <v>0.63060000000000005</v>
+        <v>0.40339999999999998</v>
       </c>
       <c r="K3" s="2">
-        <v>0.40339999999999998</v>
+        <v>0.25740000000000002</v>
       </c>
       <c r="L3" s="2">
-        <v>0.25740000000000002</v>
+        <v>0.16980000000000001</v>
       </c>
       <c r="M3" s="2">
-        <v>0.16980000000000001</v>
+        <v>0.18210000000000001</v>
       </c>
       <c r="N3" s="2">
-        <v>0.18210000000000001</v>
+        <v>0.21959999999999999</v>
       </c>
       <c r="O3" s="2">
-        <v>0.21959999999999999</v>
+        <v>0.27010000000000001</v>
       </c>
       <c r="P3" s="2">
-        <v>0.27010000000000001</v>
+        <v>0.30969999999999998</v>
       </c>
       <c r="Q3" s="2">
-        <v>0.30969999999999998</v>
+        <v>0.28010000000000002</v>
       </c>
       <c r="R3" s="2">
-        <v>0.28010000000000002</v>
+        <v>0.24779999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -4035,55 +4035,55 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>0.1603</v>
+        <v>0.19339999999999999</v>
       </c>
       <c r="C4" s="2">
-        <v>0.19339999999999999</v>
+        <v>0.20830000000000001</v>
       </c>
       <c r="D4" s="2">
-        <v>0.20830000000000001</v>
+        <v>0.17630000000000001</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17630000000000001</v>
+        <v>0.1459</v>
       </c>
       <c r="F4" s="2">
-        <v>0.1459</v>
+        <v>0.13780000000000001</v>
       </c>
       <c r="G4" s="2">
-        <v>0.13780000000000001</v>
+        <v>0.14660000000000001</v>
       </c>
       <c r="H4" s="2">
-        <v>0.14660000000000001</v>
+        <v>0.1671</v>
       </c>
       <c r="I4" s="2">
-        <v>0.1671</v>
+        <v>0.1817</v>
       </c>
       <c r="J4" s="2">
-        <v>0.1817</v>
+        <v>0.1661</v>
       </c>
       <c r="K4" s="2">
-        <v>0.1661</v>
+        <v>0.17180000000000001</v>
       </c>
       <c r="L4" s="2">
-        <v>0.17180000000000001</v>
+        <v>0.16159999999999999</v>
       </c>
       <c r="M4" s="2">
-        <v>0.16159999999999999</v>
+        <v>0.20860000000000001</v>
       </c>
       <c r="N4" s="2">
-        <v>0.20860000000000001</v>
+        <v>0.2303</v>
       </c>
       <c r="O4" s="2">
-        <v>0.2303</v>
+        <v>0.24629999999999999</v>
       </c>
       <c r="P4" s="2">
-        <v>0.24629999999999999</v>
+        <v>0.29649999999999999</v>
       </c>
       <c r="Q4" s="2">
-        <v>0.29649999999999999</v>
+        <v>0.28460000000000002</v>
       </c>
       <c r="R4" s="2">
-        <v>0.28460000000000002</v>
+        <v>0.32019999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -4091,43 +4091,43 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>5.4000000000000003E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="C5" s="2">
-        <v>5.1999999999999998E-3</v>
+        <v>4.8999999999999998E-3</v>
       </c>
       <c r="D5" s="2">
-        <v>4.8999999999999998E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="E5" s="2">
-        <v>4.1000000000000003E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="F5" s="2">
-        <v>3.0999999999999999E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="G5" s="2">
-        <v>2.3E-3</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="H5" s="2">
-        <v>1.6999999999999999E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="I5" s="2">
-        <v>1.6000000000000001E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="J5" s="2">
-        <v>1.2999999999999999E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="K5" s="2">
-        <v>1E-3</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="L5" s="2">
-        <v>6.9999999999999999E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="M5" s="2">
-        <v>5.0000000000000001E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="N5" s="2">
-        <v>4.0000000000000002E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="O5" s="2">
         <v>2.9999999999999997E-4</v>
@@ -4147,55 +4147,55 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>0.59809999999999997</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="C6" s="2">
-        <v>0.56599999999999995</v>
+        <v>0.46810000000000002</v>
       </c>
       <c r="D6" s="2">
-        <v>0.46810000000000002</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="E6" s="2">
-        <v>0.36799999999999999</v>
+        <v>0.32029999999999997</v>
       </c>
       <c r="F6" s="2">
-        <v>0.32029999999999997</v>
+        <v>0.33169999999999999</v>
       </c>
       <c r="G6" s="2">
-        <v>0.33169999999999999</v>
+        <v>0.39579999999999999</v>
       </c>
       <c r="H6" s="2">
-        <v>0.39579999999999999</v>
+        <v>0.41620000000000001</v>
       </c>
       <c r="I6" s="2">
-        <v>0.41620000000000001</v>
+        <v>0.39560000000000001</v>
       </c>
       <c r="J6" s="2">
-        <v>0.39560000000000001</v>
+        <v>0.33</v>
       </c>
       <c r="K6" s="2">
-        <v>0.33</v>
+        <v>0.27689999999999998</v>
       </c>
       <c r="L6" s="2">
-        <v>0.27689999999999998</v>
+        <v>0.2341</v>
       </c>
       <c r="M6" s="2">
-        <v>0.2341</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="N6" s="2">
-        <v>0.25700000000000001</v>
+        <v>0.26040000000000002</v>
       </c>
       <c r="O6" s="2">
-        <v>0.26040000000000002</v>
+        <v>0.24390000000000001</v>
       </c>
       <c r="P6" s="2">
-        <v>0.24390000000000001</v>
+        <v>0.25240000000000001</v>
       </c>
       <c r="Q6" s="2">
-        <v>0.25240000000000001</v>
+        <v>0.2298</v>
       </c>
       <c r="R6" s="2">
-        <v>0.2298</v>
+        <v>0.22409999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -4203,55 +4203,55 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0.43859999999999999</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="C7" s="2">
-        <v>0.42199999999999999</v>
+        <v>0.41489999999999999</v>
       </c>
       <c r="D7" s="2">
-        <v>0.41489999999999999</v>
+        <v>0.37419999999999998</v>
       </c>
       <c r="E7" s="2">
-        <v>0.37419999999999998</v>
+        <v>0.38290000000000002</v>
       </c>
       <c r="F7" s="2">
-        <v>0.38290000000000002</v>
+        <v>0.40010000000000001</v>
       </c>
       <c r="G7" s="2">
-        <v>0.40010000000000001</v>
+        <v>0.41620000000000001</v>
       </c>
       <c r="H7" s="2">
-        <v>0.41620000000000001</v>
+        <v>0.42009999999999997</v>
       </c>
       <c r="I7" s="2">
-        <v>0.42009999999999997</v>
+        <v>0.33829999999999999</v>
       </c>
       <c r="J7" s="2">
-        <v>0.33829999999999999</v>
+        <v>0.26950000000000002</v>
       </c>
       <c r="K7" s="2">
-        <v>0.26950000000000002</v>
+        <v>0.23519999999999999</v>
       </c>
       <c r="L7" s="2">
-        <v>0.23519999999999999</v>
+        <v>0.21360000000000001</v>
       </c>
       <c r="M7" s="2">
-        <v>0.21360000000000001</v>
+        <v>0.2626</v>
       </c>
       <c r="N7" s="2">
-        <v>0.2626</v>
+        <v>0.29530000000000001</v>
       </c>
       <c r="O7" s="2">
-        <v>0.29530000000000001</v>
+        <v>0.32640000000000002</v>
       </c>
       <c r="P7" s="2">
-        <v>0.32640000000000002</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="Q7" s="2">
-        <v>0.34200000000000003</v>
+        <v>0.30649999999999999</v>
       </c>
       <c r="R7" s="2">
-        <v>0.30649999999999999</v>
+        <v>0.29260000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -4259,55 +4259,55 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0</v>
+        <v>5.1400000000000001E-2</v>
       </c>
       <c r="C8" s="2">
-        <v>5.1400000000000001E-2</v>
+        <v>9.6299999999999997E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>9.6299999999999997E-2</v>
+        <v>0.4335</v>
       </c>
       <c r="E8" s="2">
-        <v>0.4335</v>
+        <v>0.62660000000000005</v>
       </c>
       <c r="F8" s="2">
-        <v>0.62660000000000005</v>
+        <v>0.68659999999999999</v>
       </c>
       <c r="G8" s="2">
-        <v>0.68659999999999999</v>
+        <v>0.64419999999999999</v>
       </c>
       <c r="H8" s="2">
-        <v>0.64419999999999999</v>
+        <v>0.28620000000000001</v>
       </c>
       <c r="I8" s="2">
-        <v>0.28620000000000001</v>
+        <v>0.16489999999999999</v>
       </c>
       <c r="J8" s="2">
-        <v>0.16489999999999999</v>
+        <v>0.1159</v>
       </c>
       <c r="K8" s="2">
-        <v>0.1159</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="L8" s="2">
-        <v>0.14099999999999999</v>
+        <v>0.1641</v>
       </c>
       <c r="M8" s="2">
-        <v>0.1641</v>
+        <v>0.16950000000000001</v>
       </c>
       <c r="N8" s="2">
-        <v>0.16950000000000001</v>
+        <v>0.16819999999999999</v>
       </c>
       <c r="O8" s="2">
-        <v>0.16819999999999999</v>
+        <v>0.16539999999999999</v>
       </c>
       <c r="P8" s="2">
-        <v>0.16539999999999999</v>
+        <v>0.14990000000000001</v>
       </c>
       <c r="Q8" s="2">
-        <v>0.14990000000000001</v>
+        <v>0.14580000000000001</v>
       </c>
       <c r="R8" s="2">
-        <v>0.14580000000000001</v>
+        <v>0.12859999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -4315,55 +4315,55 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.60529999999999995</v>
+        <v>0.59140000000000004</v>
       </c>
       <c r="C9" s="2">
-        <v>0.59140000000000004</v>
+        <v>0.58030000000000004</v>
       </c>
       <c r="D9" s="2">
-        <v>0.58030000000000004</v>
+        <v>0.5323</v>
       </c>
       <c r="E9" s="2">
-        <v>0.5323</v>
+        <v>0.4546</v>
       </c>
       <c r="F9" s="2">
-        <v>0.4546</v>
+        <v>0.38129999999999997</v>
       </c>
       <c r="G9" s="2">
-        <v>0.38129999999999997</v>
+        <v>0.30769999999999997</v>
       </c>
       <c r="H9" s="2">
-        <v>0.30769999999999997</v>
+        <v>0.26179999999999998</v>
       </c>
       <c r="I9" s="2">
-        <v>0.26179999999999998</v>
+        <v>0.22189999999999999</v>
       </c>
       <c r="J9" s="2">
-        <v>0.22189999999999999</v>
+        <v>0.1812</v>
       </c>
       <c r="K9" s="2">
-        <v>0.1812</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="L9" s="2">
-        <v>0.14499999999999999</v>
+        <v>0.1216</v>
       </c>
       <c r="M9" s="2">
-        <v>0.1216</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="N9" s="2">
-        <v>0.11700000000000001</v>
+        <v>0.1193</v>
       </c>
       <c r="O9" s="2">
-        <v>0.1193</v>
+        <v>0.1196</v>
       </c>
       <c r="P9" s="2">
-        <v>0.1196</v>
+        <v>0.1133</v>
       </c>
       <c r="Q9" s="2">
-        <v>0.1133</v>
+        <v>0.1033</v>
       </c>
       <c r="R9" s="2">
-        <v>0.1033</v>
+        <v>9.1600000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -4371,55 +4371,55 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.38650000000000001</v>
+        <v>0.35759999999999997</v>
       </c>
       <c r="C10" s="2">
-        <v>0.35759999999999997</v>
+        <v>0.32929999999999998</v>
       </c>
       <c r="D10" s="2">
-        <v>0.32929999999999998</v>
+        <v>0.2999</v>
       </c>
       <c r="E10" s="2">
-        <v>0.2999</v>
+        <v>0.26329999999999998</v>
       </c>
       <c r="F10" s="2">
-        <v>0.26329999999999998</v>
+        <v>0.24260000000000001</v>
       </c>
       <c r="G10" s="2">
-        <v>0.24260000000000001</v>
+        <v>0.2324</v>
       </c>
       <c r="H10" s="2">
-        <v>0.2324</v>
+        <v>0.23760000000000001</v>
       </c>
       <c r="I10" s="2">
-        <v>0.23760000000000001</v>
+        <v>0.24129999999999999</v>
       </c>
       <c r="J10" s="2">
-        <v>0.24129999999999999</v>
+        <v>0.2321</v>
       </c>
       <c r="K10" s="2">
-        <v>0.2321</v>
+        <v>0.21940000000000001</v>
       </c>
       <c r="L10" s="2">
-        <v>0.21940000000000001</v>
+        <v>0.1832</v>
       </c>
       <c r="M10" s="2">
-        <v>0.1832</v>
+        <v>0.17380000000000001</v>
       </c>
       <c r="N10" s="2">
-        <v>0.17380000000000001</v>
+        <v>0.17730000000000001</v>
       </c>
       <c r="O10" s="2">
-        <v>0.17730000000000001</v>
+        <v>0.18920000000000001</v>
       </c>
       <c r="P10" s="2">
-        <v>0.18920000000000001</v>
+        <v>0.20469999999999999</v>
       </c>
       <c r="Q10" s="2">
-        <v>0.20469999999999999</v>
+        <v>0.18590000000000001</v>
       </c>
       <c r="R10" s="2">
-        <v>0.18590000000000001</v>
+        <v>0.1673</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -4427,55 +4427,55 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.31640000000000001</v>
+        <v>0.29389999999999999</v>
       </c>
       <c r="C11" s="2">
-        <v>0.29389999999999999</v>
+        <v>0.25380000000000003</v>
       </c>
       <c r="D11" s="2">
-        <v>0.25380000000000003</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E11" s="2">
-        <v>0.20200000000000001</v>
+        <v>0.16339999999999999</v>
       </c>
       <c r="F11" s="2">
-        <v>0.16339999999999999</v>
+        <v>0.13009999999999999</v>
       </c>
       <c r="G11" s="2">
-        <v>0.13009999999999999</v>
+        <v>0.10440000000000001</v>
       </c>
       <c r="H11" s="2">
-        <v>0.10440000000000001</v>
+        <v>8.4500000000000006E-2</v>
       </c>
       <c r="I11" s="2">
-        <v>8.4500000000000006E-2</v>
+        <v>6.6199999999999995E-2</v>
       </c>
       <c r="J11" s="2">
-        <v>6.6199999999999995E-2</v>
+        <v>5.0700000000000002E-2</v>
       </c>
       <c r="K11" s="2">
-        <v>5.0700000000000002E-2</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="L11" s="2">
-        <v>3.6299999999999999E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="M11" s="2">
-        <v>2.52E-2</v>
+        <v>1.9699999999999999E-2</v>
       </c>
       <c r="N11" s="2">
-        <v>1.9699999999999999E-2</v>
+        <v>1.78E-2</v>
       </c>
       <c r="O11" s="2">
-        <v>1.78E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="P11" s="2">
-        <v>1.5900000000000001E-2</v>
+        <v>1.4200000000000001E-2</v>
       </c>
       <c r="Q11" s="2">
-        <v>1.4200000000000001E-2</v>
+        <v>1.1599999999999999E-2</v>
       </c>
       <c r="R11" s="2">
-        <v>1.1599999999999999E-2</v>
+        <v>1.06E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -4483,55 +4483,55 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.66400000000000003</v>
+        <v>0.64510000000000001</v>
       </c>
       <c r="C12" s="2">
-        <v>0.64510000000000001</v>
+        <v>0.57479999999999998</v>
       </c>
       <c r="D12" s="2">
-        <v>0.57479999999999998</v>
+        <v>0.53220000000000001</v>
       </c>
       <c r="E12" s="2">
-        <v>0.53220000000000001</v>
+        <v>0.4153</v>
       </c>
       <c r="F12" s="2">
-        <v>0.4153</v>
+        <v>0.3715</v>
       </c>
       <c r="G12" s="2">
-        <v>0.3715</v>
+        <v>0.33129999999999998</v>
       </c>
       <c r="H12" s="2">
-        <v>0.33129999999999998</v>
+        <v>0.32719999999999999</v>
       </c>
       <c r="I12" s="2">
-        <v>0.32719999999999999</v>
+        <v>0.36549999999999999</v>
       </c>
       <c r="J12" s="2">
-        <v>0.36549999999999999</v>
+        <v>0.40579999999999999</v>
       </c>
       <c r="K12" s="2">
-        <v>0.40579999999999999</v>
+        <v>0.44440000000000002</v>
       </c>
       <c r="L12" s="2">
-        <v>0.44440000000000002</v>
+        <v>0.4118</v>
       </c>
       <c r="M12" s="2">
-        <v>0.4118</v>
+        <v>0.44479999999999997</v>
       </c>
       <c r="N12" s="2">
-        <v>0.44479999999999997</v>
+        <v>0.41770000000000002</v>
       </c>
       <c r="O12" s="2">
-        <v>0.41770000000000002</v>
+        <v>0.4007</v>
       </c>
       <c r="P12" s="2">
-        <v>0.4007</v>
+        <v>0.40179999999999999</v>
       </c>
       <c r="Q12" s="2">
-        <v>0.40179999999999999</v>
+        <v>0.3175</v>
       </c>
       <c r="R12" s="2">
-        <v>0.3175</v>
+        <v>0.2651</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -4539,55 +4539,55 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.69479999999999997</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="C13" s="2">
-        <v>0.42299999999999999</v>
+        <v>0.3296</v>
       </c>
       <c r="D13" s="2">
-        <v>0.3296</v>
+        <v>0.28549999999999998</v>
       </c>
       <c r="E13" s="2">
-        <v>0.28549999999999998</v>
+        <v>0.46010000000000001</v>
       </c>
       <c r="F13" s="2">
-        <v>0.46010000000000001</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="G13" s="2">
-        <v>0.53900000000000003</v>
+        <v>0.63349999999999995</v>
       </c>
       <c r="H13" s="2">
-        <v>0.63349999999999995</v>
+        <v>0.59970000000000001</v>
       </c>
       <c r="I13" s="2">
-        <v>0.59970000000000001</v>
+        <v>0.42120000000000002</v>
       </c>
       <c r="J13" s="2">
-        <v>0.42120000000000002</v>
+        <v>0.36820000000000003</v>
       </c>
       <c r="K13" s="2">
-        <v>0.36820000000000003</v>
+        <v>0.32669999999999999</v>
       </c>
       <c r="L13" s="2">
-        <v>0.32669999999999999</v>
+        <v>0.32979999999999998</v>
       </c>
       <c r="M13" s="2">
-        <v>0.32979999999999998</v>
+        <v>0.32969999999999999</v>
       </c>
       <c r="N13" s="2">
-        <v>0.32969999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="O13" s="2">
-        <v>0.31</v>
+        <v>0.26190000000000002</v>
       </c>
       <c r="P13" s="2">
-        <v>0.26190000000000002</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="Q13" s="2">
-        <v>0.20699999999999999</v>
+        <v>0.14729999999999999</v>
       </c>
       <c r="R13" s="2">
-        <v>0.14729999999999999</v>
+        <v>0.1075</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -4595,55 +4595,55 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>1.2688999999999999</v>
+        <v>0.71740000000000004</v>
       </c>
       <c r="C14" s="2">
-        <v>0.71740000000000004</v>
+        <v>0.64670000000000005</v>
       </c>
       <c r="D14" s="2">
-        <v>0.64670000000000005</v>
+        <v>0.53349999999999997</v>
       </c>
       <c r="E14" s="2">
-        <v>0.53349999999999997</v>
+        <v>0.48820000000000002</v>
       </c>
       <c r="F14" s="2">
-        <v>0.48820000000000002</v>
+        <v>0.48049999999999998</v>
       </c>
       <c r="G14" s="2">
-        <v>0.48049999999999998</v>
+        <v>0.47770000000000001</v>
       </c>
       <c r="H14" s="2">
-        <v>0.47770000000000001</v>
+        <v>0.44469999999999998</v>
       </c>
       <c r="I14" s="2">
-        <v>0.44469999999999998</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="J14" s="2">
-        <v>0.39300000000000002</v>
+        <v>0.30220000000000002</v>
       </c>
       <c r="K14" s="2">
-        <v>0.30220000000000002</v>
+        <v>0.2631</v>
       </c>
       <c r="L14" s="2">
-        <v>0.2631</v>
+        <v>0.2167</v>
       </c>
       <c r="M14" s="2">
-        <v>0.2167</v>
+        <v>0.25690000000000002</v>
       </c>
       <c r="N14" s="2">
-        <v>0.25690000000000002</v>
+        <v>0.27229999999999999</v>
       </c>
       <c r="O14" s="2">
-        <v>0.27229999999999999</v>
+        <v>0.3266</v>
       </c>
       <c r="P14" s="2">
-        <v>0.3266</v>
+        <v>0.33839999999999998</v>
       </c>
       <c r="Q14" s="2">
-        <v>0.33839999999999998</v>
+        <v>0.30570000000000003</v>
       </c>
       <c r="R14" s="2">
-        <v>0.30570000000000003</v>
+        <v>0.25950000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -4686,20 +4686,20 @@
       <c r="M15" t="s">
         <v>15</v>
       </c>
-      <c r="N15" t="s">
-        <v>15</v>
-      </c>
-      <c r="O15">
+      <c r="N15" s="2">
         <v>0.63460000000000005</v>
       </c>
+      <c r="O15" s="2">
+        <v>0.40489999999999998</v>
+      </c>
       <c r="P15" s="2">
-        <v>0.40489999999999998</v>
+        <v>0.30259999999999998</v>
       </c>
       <c r="Q15" s="2">
-        <v>0.30259999999999998</v>
+        <v>0.30669999999999997</v>
       </c>
       <c r="R15" s="2">
-        <v>0.30669999999999997</v>
+        <v>0.30790000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -4707,55 +4707,55 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>0.193</v>
+        <v>0.24660000000000001</v>
       </c>
       <c r="C16" s="2">
-        <v>0.24660000000000001</v>
+        <v>0.27539999999999998</v>
       </c>
       <c r="D16" s="2">
-        <v>0.27539999999999998</v>
+        <v>0.32169999999999999</v>
       </c>
       <c r="E16" s="2">
-        <v>0.32169999999999999</v>
+        <v>0.3377</v>
       </c>
       <c r="F16" s="2">
-        <v>0.3377</v>
+        <v>0.3866</v>
       </c>
       <c r="G16" s="2">
-        <v>0.3866</v>
+        <v>0.39939999999999998</v>
       </c>
       <c r="H16" s="2">
-        <v>0.39939999999999998</v>
+        <v>0.38159999999999999</v>
       </c>
       <c r="I16" s="2">
-        <v>0.38159999999999999</v>
+        <v>0.3347</v>
       </c>
       <c r="J16" s="2">
-        <v>0.3347</v>
+        <v>0.2792</v>
       </c>
       <c r="K16" s="2">
-        <v>0.2792</v>
+        <v>0.2437</v>
       </c>
       <c r="L16" s="2">
-        <v>0.2437</v>
+        <v>0.192</v>
       </c>
       <c r="M16" s="2">
-        <v>0.192</v>
+        <v>0.20979999999999999</v>
       </c>
       <c r="N16" s="2">
-        <v>0.20979999999999999</v>
+        <v>0.25159999999999999</v>
       </c>
       <c r="O16" s="2">
-        <v>0.25159999999999999</v>
+        <v>0.27629999999999999</v>
       </c>
       <c r="P16" s="2">
-        <v>0.27629999999999999</v>
+        <v>0.3105</v>
       </c>
       <c r="Q16" s="2">
-        <v>0.3105</v>
+        <v>0.28270000000000001</v>
       </c>
       <c r="R16" s="2">
-        <v>0.28270000000000001</v>
+        <v>0.26469999999999999</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">
@@ -4771,8 +4771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E356A6A6-24A0-42A0-8188-ED9E5DA792BF}">
   <dimension ref="B33:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update 2020-03-21 06:45 issue with missing contries corrected
</commit_message>
<xml_diff>
--- a/COVID-19 Apps/Growth Chart.xlsx
+++ b/COVID-19 Apps/Growth Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zur Bonsen Georg\Documents\Programme\Beyond4P_Apps\COVID-19 Apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE760A5-2077-4027-B8BD-B87D4B18EF8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD349332-0863-4F77-AC3D-5CDD68CFC101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{A4C1FE6B-DE9B-48BC-897C-015B097916DC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Country/Region</t>
   </si>
@@ -81,9 +81,6 @@
     <t>US</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>United Kingdom</t>
   </si>
   <si>
@@ -169,6 +166,57 @@
   </si>
   <si>
     <t>This algorithm smoothens out short term discontinuities, e.g. reporting outages or peaks</t>
+  </si>
+  <si>
+    <t>2020-03-05</t>
+  </si>
+  <si>
+    <t>2020-03-06</t>
+  </si>
+  <si>
+    <t>2020-03-07</t>
+  </si>
+  <si>
+    <t>2020-03-08</t>
+  </si>
+  <si>
+    <t>2020-03-09</t>
+  </si>
+  <si>
+    <t>2020-03-10</t>
+  </si>
+  <si>
+    <t>2020-03-11</t>
+  </si>
+  <si>
+    <t>2020-03-12</t>
+  </si>
+  <si>
+    <t>2020-03-13</t>
+  </si>
+  <si>
+    <t>2020-03-14</t>
+  </si>
+  <si>
+    <t>2020-03-15</t>
+  </si>
+  <si>
+    <t>2020-03-16</t>
+  </si>
+  <si>
+    <t>2020-03-17</t>
+  </si>
+  <si>
+    <t>2020-03-18</t>
+  </si>
+  <si>
+    <t>2020-03-19</t>
+  </si>
+  <si>
+    <t>2020-03-20</t>
+  </si>
+  <si>
+    <t>Last Trend</t>
   </si>
 </sst>
 </file>
@@ -271,9 +319,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -414,121 +461,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$2:$R$2</c:f>
+              <c:f>TABLE!$F$2:$V$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.55569999999999997</c:v>
+                  <c:v>0.3677823999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60429999999999995</c:v>
+                  <c:v>0.321391592</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4592</c:v>
+                  <c:v>0.34800202549999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36780000000000002</c:v>
+                  <c:v>0.3677823999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32140000000000002</c:v>
+                  <c:v>0.36292533300000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34799999999999998</c:v>
+                  <c:v>0.35147031379999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36780000000000002</c:v>
+                  <c:v>0.33688312009999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3629</c:v>
+                  <c:v>0.32338581659999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.35149999999999998</c:v>
+                  <c:v>0.35291814960000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33689999999999998</c:v>
+                  <c:v>0.36813369880000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.32340000000000002</c:v>
+                  <c:v>0.37857731509999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.35289999999999999</c:v>
+                  <c:v>0.36482849899999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.36809999999999998</c:v>
+                  <c:v>0.32166784199999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.37859999999999999</c:v>
+                  <c:v>0.28600843129999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.36480000000000001</c:v>
+                  <c:v>0.25389974119999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.32169999999999999</c:v>
+                  <c:v>0.2430144997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28599999999999998</c:v>
+                  <c:v>0.1862891207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -567,121 +613,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$3:$R$3</c:f>
+              <c:f>TABLE!$F$3:$V$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.38379999999999997</c:v>
+                  <c:v>1.1533251606999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66400000000000003</c:v>
+                  <c:v>1.0168317783</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95699999999999996</c:v>
+                  <c:v>0.94328501570000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1533</c:v>
+                  <c:v>0.81548976559999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0167999999999999</c:v>
+                  <c:v>0.63061443279999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94330000000000003</c:v>
+                  <c:v>0.40340599780000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8155</c:v>
+                  <c:v>0.25743342969999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63060000000000005</c:v>
+                  <c:v>0.1697654358</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40339999999999998</c:v>
+                  <c:v>0.1820525519</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.25740000000000002</c:v>
+                  <c:v>0.2196046797</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16980000000000001</c:v>
+                  <c:v>0.2701211288</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.18210000000000001</c:v>
+                  <c:v>0.30965515259999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.21959999999999999</c:v>
+                  <c:v>0.2800673964</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27010000000000001</c:v>
+                  <c:v>0.24782467380000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.30969999999999998</c:v>
+                  <c:v>0.20665202290000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.28010000000000002</c:v>
+                  <c:v>0.20427459049999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.24779999999999999</c:v>
+                  <c:v>0.2573816156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,121 +765,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$4:$R$4</c:f>
+              <c:f>TABLE!$F$4:$V$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.19339999999999999</c:v>
+                  <c:v>0.14589019049999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20830000000000001</c:v>
+                  <c:v>0.13781630559999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17630000000000001</c:v>
+                  <c:v>0.1465968761</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1459</c:v>
+                  <c:v>0.16712800620000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13780000000000001</c:v>
+                  <c:v>0.18170385650000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.14660000000000001</c:v>
+                  <c:v>0.16605471629999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1671</c:v>
+                  <c:v>0.17184176600000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1817</c:v>
+                  <c:v>0.16155366139999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1661</c:v>
+                  <c:v>0.2085501589</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17180000000000001</c:v>
+                  <c:v>0.23027433420000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16159999999999999</c:v>
+                  <c:v>0.24633237459999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20860000000000001</c:v>
+                  <c:v>0.29652201369999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2303</c:v>
+                  <c:v>0.28464799909999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.24629999999999999</c:v>
+                  <c:v>0.32018916330000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.29649999999999999</c:v>
+                  <c:v>0.31572953599999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.28460000000000002</c:v>
+                  <c:v>0.28908151319999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32019999999999998</c:v>
+                  <c:v>0.17951959540000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,121 +917,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$5:$R$5</c:f>
+              <c:f>TABLE!$F$5:$V$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>5.1999999999999998E-3</c:v>
+                  <c:v>3.1003719000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8999999999999998E-3</c:v>
+                  <c:v>2.2778988999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1000000000000003E-3</c:v>
+                  <c:v>1.7306236999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0999999999999999E-3</c:v>
+                  <c:v>1.5537938E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3E-3</c:v>
+                  <c:v>1.3127983000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6999999999999999E-3</c:v>
+                  <c:v>9.8875250000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6000000000000001E-3</c:v>
+                  <c:v>6.9247079999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2999999999999999E-3</c:v>
+                  <c:v>4.7122279999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.5554940000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9999999999999999E-4</c:v>
+                  <c:v>2.9257060000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0000000000000001E-4</c:v>
+                  <c:v>2.6465990000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.0000000000000002E-4</c:v>
+                  <c:v>2.8104649999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.9999999999999997E-4</c:v>
+                  <c:v>3.0464089999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9999999999999997E-4</c:v>
+                  <c:v>3.4879259999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.9999999999999997E-4</c:v>
+                  <c:v>4.0214489999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.9999999999999997E-4</c:v>
+                  <c:v>5.0884349999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.9999999999999997E-4</c:v>
+                  <c:v>1.1582630999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,121 +1070,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$6:$R$6</c:f>
+              <c:f>TABLE!$F$6:$V$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.56599999999999995</c:v>
+                  <c:v>0.32025751149999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46810000000000002</c:v>
+                  <c:v>0.33168489089999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36799999999999999</c:v>
+                  <c:v>0.3958443687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32029999999999997</c:v>
+                  <c:v>0.41615075730000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33169999999999999</c:v>
+                  <c:v>0.39560415570000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39579999999999999</c:v>
+                  <c:v>0.3300156065</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.41620000000000001</c:v>
+                  <c:v>0.27694342189999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39560000000000001</c:v>
+                  <c:v>0.23411115230000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33</c:v>
+                  <c:v>0.25697703849999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.27689999999999998</c:v>
+                  <c:v>0.26038224300000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2341</c:v>
+                  <c:v>0.24394108680000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.25700000000000001</c:v>
+                  <c:v>0.2524307536</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.26040000000000002</c:v>
+                  <c:v>0.2298135389</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.24390000000000001</c:v>
+                  <c:v>0.22407073459999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.25240000000000001</c:v>
+                  <c:v>0.2161058199</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2298</c:v>
+                  <c:v>0.20246639390000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.22409999999999999</c:v>
+                  <c:v>0.16251027679999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1180,121 +1222,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$7:$R$7</c:f>
+              <c:f>TABLE!$F$7:$V$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.42199999999999999</c:v>
+                  <c:v>0.38292517469999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41489999999999999</c:v>
+                  <c:v>0.40007208849999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37419999999999998</c:v>
+                  <c:v>0.41621399809999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38290000000000002</c:v>
+                  <c:v>0.42005077870000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.40010000000000001</c:v>
+                  <c:v>0.33825805390000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.41620000000000001</c:v>
+                  <c:v>0.2695297418</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.42009999999999997</c:v>
+                  <c:v>0.235160965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33829999999999999</c:v>
+                  <c:v>0.2136247322</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.26950000000000002</c:v>
+                  <c:v>0.26255276249999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23519999999999999</c:v>
+                  <c:v>0.2952508915</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.21360000000000001</c:v>
+                  <c:v>0.32638571830000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2626</c:v>
+                  <c:v>0.34195791479999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.29530000000000001</c:v>
+                  <c:v>0.30653677369999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.32640000000000002</c:v>
+                  <c:v>0.29255758450000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.34200000000000003</c:v>
+                  <c:v>0.27294795560000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.30649999999999999</c:v>
+                  <c:v>0.28074743070000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.29260000000000003</c:v>
+                  <c:v>0.29556135770000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1333,121 +1374,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$8:$R$8</c:f>
+              <c:f>TABLE!$F$8:$V$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>5.1400000000000001E-2</c:v>
+                  <c:v>0.62657656169999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6299999999999997E-2</c:v>
+                  <c:v>0.68655042489999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4335</c:v>
+                  <c:v>0.64416372899999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.62660000000000005</c:v>
+                  <c:v>0.28621164030000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68659999999999999</c:v>
+                  <c:v>0.16487509440000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.64419999999999999</c:v>
+                  <c:v>0.115892272</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.28620000000000001</c:v>
+                  <c:v>0.1409735262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16489999999999999</c:v>
+                  <c:v>0.1641260481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1159</c:v>
+                  <c:v>0.16950056550000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14099999999999999</c:v>
+                  <c:v>0.16819006719999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1641</c:v>
+                  <c:v>0.16542047360000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16950000000000001</c:v>
+                  <c:v>0.14994819240000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16819999999999999</c:v>
+                  <c:v>0.1457845639</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.16539999999999999</c:v>
+                  <c:v>0.1286277726</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.14990000000000001</c:v>
+                  <c:v>0.13449389549999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.14580000000000001</c:v>
+                  <c:v>0.15480856030000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.12859999999999999</c:v>
+                  <c:v>0.25773195879999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1488,121 +1528,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$9:$R$9</c:f>
+              <c:f>TABLE!$F$9:$V$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.59140000000000004</c:v>
+                  <c:v>0.4546337802</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58030000000000004</c:v>
+                  <c:v>0.3812572454</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5323</c:v>
+                  <c:v>0.30774997970000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4546</c:v>
+                  <c:v>0.26184715180000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38129999999999997</c:v>
+                  <c:v>0.22186834220000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30769999999999997</c:v>
+                  <c:v>0.18121716099999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26179999999999998</c:v>
+                  <c:v>0.14496841220000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.22189999999999999</c:v>
+                  <c:v>0.12158720670000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1812</c:v>
+                  <c:v>0.1170456064</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14499999999999999</c:v>
+                  <c:v>0.11929681960000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1216</c:v>
+                  <c:v>0.11961094680000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.11700000000000001</c:v>
+                  <c:v>0.1133050874</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1193</c:v>
+                  <c:v>0.1032697875</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1196</c:v>
+                  <c:v>9.1635237699999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1133</c:v>
+                  <c:v>8.1022613199999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1033</c:v>
+                  <c:v>7.3930934700000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.1600000000000001E-2</c:v>
+                  <c:v>6.7202694600000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1641,121 +1680,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$10:$R$10</c:f>
+              <c:f>TABLE!$F$10:$V$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.35759999999999997</c:v>
+                  <c:v>0.26328978619999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32929999999999998</c:v>
+                  <c:v>0.242627288</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2999</c:v>
+                  <c:v>0.23242417000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26329999999999998</c:v>
+                  <c:v>0.23762314239999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.24260000000000001</c:v>
+                  <c:v>0.2412545576</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2324</c:v>
+                  <c:v>0.2321292975</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23760000000000001</c:v>
+                  <c:v>0.21935918439999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24129999999999999</c:v>
+                  <c:v>0.18322236650000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2321</c:v>
+                  <c:v>0.17382754080000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.21940000000000001</c:v>
+                  <c:v>0.1772625759</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1832</c:v>
+                  <c:v>0.1891977608</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.17380000000000001</c:v>
+                  <c:v>0.20474288769999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.17730000000000001</c:v>
+                  <c:v>0.1859297228</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.18920000000000001</c:v>
+                  <c:v>0.16727506880000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.20469999999999999</c:v>
+                  <c:v>0.1423736665</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.18590000000000001</c:v>
+                  <c:v>0.13766754959999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1673</c:v>
+                  <c:v>0.14587547219999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1796,121 +1834,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$11:$R$11</c:f>
+              <c:f>TABLE!$F$11:$V$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.29389999999999999</c:v>
+                  <c:v>0.16337974129999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25380000000000003</c:v>
+                  <c:v>0.13009966749999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20200000000000001</c:v>
+                  <c:v>0.10440006759999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16339999999999999</c:v>
+                  <c:v>8.4525657300000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13009999999999999</c:v>
+                  <c:v>6.6200310499999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10440000000000001</c:v>
+                  <c:v>5.06931942E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.4500000000000006E-2</c:v>
+                  <c:v>3.6307210899999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.6199999999999995E-2</c:v>
+                  <c:v>2.5158744E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0700000000000002E-2</c:v>
+                  <c:v>1.96789359E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.6299999999999999E-2</c:v>
+                  <c:v>1.77784821E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.52E-2</c:v>
+                  <c:v>1.58945983E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9699999999999999E-2</c:v>
+                  <c:v>1.4247231799999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.78E-2</c:v>
+                  <c:v>1.16063117E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5900000000000001E-2</c:v>
+                  <c:v>1.0639959399999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.4200000000000001E-2</c:v>
+                  <c:v>1.08730939E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1599999999999999E-2</c:v>
+                  <c:v>1.15015645E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.06E-2</c:v>
+                  <c:v>1.0157618199999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1952,121 +1989,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$12:$R$12</c:f>
+              <c:f>TABLE!$F$12:$V$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.64510000000000001</c:v>
+                  <c:v>0.41531027790000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57479999999999998</c:v>
+                  <c:v>0.37149472109999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53220000000000001</c:v>
+                  <c:v>0.33126424360000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4153</c:v>
+                  <c:v>0.3271811074</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3715</c:v>
+                  <c:v>0.36550818750000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.33129999999999998</c:v>
+                  <c:v>0.40581182170000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.32719999999999999</c:v>
+                  <c:v>0.44442312779999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.36549999999999999</c:v>
+                  <c:v>0.41179113499999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40579999999999999</c:v>
+                  <c:v>0.44477049810000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44440000000000002</c:v>
+                  <c:v>0.4176940998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4118</c:v>
+                  <c:v>0.40072411130000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.44479999999999997</c:v>
+                  <c:v>0.40181660079999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.41770000000000002</c:v>
+                  <c:v>0.31752852500000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.4007</c:v>
+                  <c:v>0.26505322879999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.40179999999999999</c:v>
+                  <c:v>0.22421023840000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.3175</c:v>
+                  <c:v>0.21323881149999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.2651</c:v>
+                  <c:v>0.1362244614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2105,121 +2141,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$13:$R$13</c:f>
+              <c:f>TABLE!$F$13:$V$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.42299999999999999</c:v>
+                  <c:v>0.46013943289999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3296</c:v>
+                  <c:v>0.53899069779999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28549999999999998</c:v>
+                  <c:v>0.63350323320000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46010000000000001</c:v>
+                  <c:v>0.59973722620000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53900000000000003</c:v>
+                  <c:v>0.42123220750000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.63349999999999995</c:v>
+                  <c:v>0.36820697930000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59970000000000001</c:v>
+                  <c:v>0.32672642299999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.42120000000000002</c:v>
+                  <c:v>0.32977408000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36820000000000003</c:v>
+                  <c:v>0.329660866</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32669999999999999</c:v>
+                  <c:v>0.31004561619999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.32979999999999998</c:v>
+                  <c:v>0.26191248880000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32969999999999999</c:v>
+                  <c:v>0.20700169169999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.31</c:v>
+                  <c:v>0.14734001560000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26190000000000002</c:v>
+                  <c:v>0.1075355721</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.20699999999999999</c:v>
+                  <c:v>8.7215216700000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.14729999999999999</c:v>
+                  <c:v>9.0053740600000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1075</c:v>
+                  <c:v>0.13898540649999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2262,121 +2297,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$14:$R$14</c:f>
+              <c:f>TABLE!$F$14:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.71740000000000004</c:v>
+                  <c:v>0.48824478560000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64670000000000005</c:v>
+                  <c:v>0.4805199275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53349999999999997</c:v>
+                  <c:v>0.4776924749</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48820000000000002</c:v>
+                  <c:v>0.44471277510000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48049999999999998</c:v>
+                  <c:v>0.39300391169999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47770000000000001</c:v>
+                  <c:v>0.3022130596</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44469999999999998</c:v>
+                  <c:v>0.26309155150000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39300000000000002</c:v>
+                  <c:v>0.21673258179999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.30220000000000002</c:v>
+                  <c:v>0.25685504809999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2631</c:v>
+                  <c:v>0.2723351389</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2167</c:v>
+                  <c:v>0.32657515079999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.25690000000000002</c:v>
+                  <c:v>0.33835293729999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27229999999999999</c:v>
+                  <c:v>0.30567088650000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.3266</c:v>
+                  <c:v>0.25954379259999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.33839999999999998</c:v>
+                  <c:v>0.20188107720000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.30570000000000003</c:v>
+                  <c:v>0.2112739595</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.25950000000000001</c:v>
+                  <c:v>0.29914110430000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2419,121 +2453,87 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$15:$R$15</c:f>
+              <c:f>TABLE!$F$15:$V$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00%">
-                  <c:v>0.63460000000000005</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.00%">
-                  <c:v>0.40489999999999998</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.00%">
-                  <c:v>0.30259999999999998</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.00%">
-                  <c:v>0.30669999999999997</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.00%">
-                  <c:v>0.30790000000000001</c:v>
+                  <c:v>0.30256569989999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.3067050603</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.30788612440000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.35525000499999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.39493777159999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.39829512049999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2575,121 +2575,120 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>TABLE!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+            <c:strRef>
+              <c:f>TABLE!$F$1:$V$1</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43892</c:v>
+                  <c:v>2020-03-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43893</c:v>
+                  <c:v>2020-03-06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43894</c:v>
+                  <c:v>2020-03-07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43895</c:v>
+                  <c:v>2020-03-08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43896</c:v>
+                  <c:v>2020-03-09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43897</c:v>
+                  <c:v>2020-03-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43898</c:v>
+                  <c:v>2020-03-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43899</c:v>
+                  <c:v>2020-03-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43900</c:v>
+                  <c:v>2020-03-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43901</c:v>
+                  <c:v>2020-03-14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43902</c:v>
+                  <c:v>2020-03-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43903</c:v>
+                  <c:v>2020-03-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43904</c:v>
+                  <c:v>2020-03-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43905</c:v>
+                  <c:v>2020-03-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43906</c:v>
+                  <c:v>2020-03-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43907</c:v>
+                  <c:v>2020-03-20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43908</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Last Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TABLE!$B$16:$R$16</c:f>
+              <c:f>TABLE!$F$16:$V$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.24660000000000001</c:v>
+                  <c:v>0.3377450649</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27539999999999998</c:v>
+                  <c:v>0.38663281189999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32169999999999999</c:v>
+                  <c:v>0.3993659752</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3377</c:v>
+                  <c:v>0.38164545290000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3866</c:v>
+                  <c:v>0.33474639340000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39939999999999998</c:v>
+                  <c:v>0.27919351069999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.38159999999999999</c:v>
+                  <c:v>0.24365305500000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3347</c:v>
+                  <c:v>0.1919631175</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2792</c:v>
+                  <c:v>0.20977115539999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2437</c:v>
+                  <c:v>0.25161929970000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.192</c:v>
+                  <c:v>0.27627208380000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20979999999999999</c:v>
+                  <c:v>0.31047898229999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25159999999999999</c:v>
+                  <c:v>0.28268829359999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27629999999999999</c:v>
+                  <c:v>0.26471584190000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.3105</c:v>
+                  <c:v>0.24043311000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.28270000000000001</c:v>
+                  <c:v>0.24989998799999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.26469999999999999</c:v>
+                  <c:v>0.47790868920000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2713,14 +2712,14 @@
         <c:axId val="350511704"/>
         <c:axId val="350508424"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="350511704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2760,9 +2759,10 @@
         <c:crossAx val="350508424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="350508424"/>
         <c:scaling>
@@ -3854,912 +3854,890 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50CEFAE-1AD4-44A1-9917-42DDA6C5C118}">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:R16"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>43892</v>
-      </c>
-      <c r="C1" s="1">
-        <v>43893</v>
-      </c>
-      <c r="D1" s="1">
-        <v>43894</v>
-      </c>
-      <c r="E1" s="1">
-        <v>43895</v>
-      </c>
-      <c r="F1" s="1">
-        <v>43896</v>
-      </c>
-      <c r="G1" s="1">
-        <v>43897</v>
-      </c>
-      <c r="H1" s="1">
-        <v>43898</v>
-      </c>
-      <c r="I1" s="1">
-        <v>43899</v>
-      </c>
-      <c r="J1" s="1">
-        <v>43900</v>
-      </c>
-      <c r="K1" s="1">
-        <v>43901</v>
-      </c>
-      <c r="L1" s="1">
-        <v>43902</v>
-      </c>
-      <c r="M1" s="1">
-        <v>43903</v>
-      </c>
-      <c r="N1" s="1">
-        <v>43904</v>
-      </c>
-      <c r="O1" s="1">
-        <v>43905</v>
-      </c>
-      <c r="P1" s="1">
-        <v>43906</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>43907</v>
-      </c>
-      <c r="R1" s="1">
-        <v>43908</v>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.55569999999999997</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.60429999999999995</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.4592</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.36780000000000002</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.32140000000000002</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.36780000000000002</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.3629</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.35149999999999998</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0.33689999999999998</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.32340000000000002</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0.35289999999999999</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0.36809999999999998</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0.37859999999999999</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0.36480000000000001</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0.32169999999999999</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0.28599999999999998</v>
+      <c r="F2" s="1">
+        <v>0.3677823999</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.321391592</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.34800202549999998</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.3677823999</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.36292533300000002</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.35147031379999999</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.33688312009999999</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.32338581659999999</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.35291814960000001</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.36813369880000002</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0.37857731509999998</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0.36482849899999997</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.32166784199999998</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0.28600843129999998</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0.25389974119999997</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0.2430144997</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0.1862891207</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.38379999999999997</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.66400000000000003</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.1533</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.0167999999999999</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.94330000000000003</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0.8155</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.63060000000000005</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.40339999999999998</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0.25740000000000002</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0.16980000000000001</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.18210000000000001</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.21959999999999999</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0.27010000000000001</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0.30969999999999998</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0.28010000000000002</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0.24779999999999999</v>
+      <c r="F3" s="1">
+        <v>1.1533251606999999</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.0168317783</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.94328501570000001</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.81548976559999997</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.63061443279999996</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.40340599780000003</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.25743342969999999</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.1697654358</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.1820525519</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.2196046797</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.2701211288</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.30965515259999998</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.2800673964</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0.24782467380000001</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0.20665202290000001</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0.20427459049999999</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0.2573816156</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.19339999999999999</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.20830000000000001</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.17630000000000001</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.1459</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.13780000000000001</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.14660000000000001</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.1671</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.1817</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.1661</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0.17180000000000001</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.16159999999999999</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.20860000000000001</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0.2303</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0.24629999999999999</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0.29649999999999999</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0.28460000000000002</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.32019999999999998</v>
+      <c r="F4" s="1">
+        <v>0.14589019049999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.13781630559999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.1465968761</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.16712800620000001</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.18170385650000001</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.16605471629999999</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.17184176600000001</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.16155366139999999</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.2085501589</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.23027433420000001</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.24633237459999999</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0.29652201369999998</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0.28464799909999999</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0.32018916330000002</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0.31572953599999998</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0.28908151319999997</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0.17951959540000001</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>5.1999999999999998E-3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>4.8999999999999998E-3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4.1000000000000003E-3</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2.3E-3</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K5" s="2">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="L5" s="2">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="M5" s="2">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="N5" s="2">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="O5" s="2">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="P5" s="2">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="R5" s="2">
-        <v>2.9999999999999997E-4</v>
+      <c r="F5" s="1">
+        <v>3.1003719000000001E-3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.2778988999999999E-3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.7306236999999999E-3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.5537938E-3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.3127983000000001E-3</v>
+      </c>
+      <c r="K5" s="1">
+        <v>9.8875250000000003E-4</v>
+      </c>
+      <c r="L5" s="1">
+        <v>6.9247079999999999E-4</v>
+      </c>
+      <c r="M5" s="1">
+        <v>4.7122279999999998E-4</v>
+      </c>
+      <c r="N5" s="1">
+        <v>3.5554940000000001E-4</v>
+      </c>
+      <c r="O5" s="1">
+        <v>2.9257060000000001E-4</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2.6465990000000002E-4</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>2.8104649999999997E-4</v>
+      </c>
+      <c r="R5" s="1">
+        <v>3.0464089999999999E-4</v>
+      </c>
+      <c r="S5" s="1">
+        <v>3.4879259999999999E-4</v>
+      </c>
+      <c r="T5" s="1">
+        <v>4.0214489999999999E-4</v>
+      </c>
+      <c r="U5" s="1">
+        <v>5.0884349999999999E-4</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1.1582630999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.46810000000000002</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.32029999999999997</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.33169999999999999</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.39579999999999999</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.41620000000000001</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.39560000000000001</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0.27689999999999998</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0.2341</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0.26040000000000002</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0.24390000000000001</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0.25240000000000001</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0.2298</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0.22409999999999999</v>
+      <c r="F6" s="1">
+        <v>0.32025751149999998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.33168489089999997</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.3958443687</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.41615075730000001</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.39560415570000002</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.3300156065</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.27694342189999999</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.23411115230000001</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.25697703849999998</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.26038224300000001</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0.24394108680000001</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.2524307536</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.2298135389</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0.22407073459999999</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0.2161058199</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0.20246639390000001</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0.16251027679999999</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.42199999999999999</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.41489999999999999</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.37419999999999998</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.38290000000000002</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.40010000000000001</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.41620000000000001</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.42009999999999997</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.33829999999999999</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.26950000000000002</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0.23519999999999999</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0.21360000000000001</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0.2626</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.29530000000000001</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0.32640000000000002</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0.30649999999999999</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0.29260000000000003</v>
+      <c r="F7" s="1">
+        <v>0.38292517469999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.40007208849999998</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.41621399809999998</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.42005077870000002</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.33825805390000002</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.2695297418</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.235160965</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.2136247322</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.26255276249999998</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.2952508915</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.32638571830000002</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0.34195791479999998</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.30653677369999999</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.29255758450000002</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0.27294795560000001</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0.28074743070000002</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.29556135770000003</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>5.1400000000000001E-2</v>
-      </c>
-      <c r="C8" s="2">
-        <v>9.6299999999999997E-2</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.4335</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.62660000000000005</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.68659999999999999</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.64419999999999999</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.28620000000000001</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.16489999999999999</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.1159</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0.1641</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0.16950000000000001</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0.16819999999999999</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0.16539999999999999</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0.14990000000000001</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>0.14580000000000001</v>
-      </c>
-      <c r="R8" s="2">
-        <v>0.12859999999999999</v>
+      <c r="F8" s="1">
+        <v>0.62657656169999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.68655042489999996</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.64416372899999996</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.28621164030000001</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.16487509440000001</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.115892272</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.1409735262</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.1641260481</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.16950056550000001</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.16819006719999999</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0.16542047360000001</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.14994819240000001</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.1457845639</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0.1286277726</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0.13449389549999999</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0.15480856030000001</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0.25773195879999999</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.59140000000000004</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.58030000000000004</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.5323</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.4546</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.38129999999999997</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.30769999999999997</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.26179999999999998</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.22189999999999999</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.1812</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0.1216</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0.1193</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0.1196</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0.1133</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>0.1033</v>
-      </c>
-      <c r="R9" s="2">
-        <v>9.1600000000000001E-2</v>
+      <c r="F9" s="1">
+        <v>0.4546337802</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.3812572454</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.30774997970000001</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.26184715180000001</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.22186834220000001</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.18121716099999999</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.14496841220000001</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.12158720670000001</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0.1170456064</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.11929681960000001</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.11961094680000001</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.1133050874</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.1032697875</v>
+      </c>
+      <c r="S9" s="1">
+        <v>9.1635237699999997E-2</v>
+      </c>
+      <c r="T9" s="1">
+        <v>8.1022613199999996E-2</v>
+      </c>
+      <c r="U9" s="1">
+        <v>7.3930934700000006E-2</v>
+      </c>
+      <c r="V9" s="1">
+        <v>6.7202694600000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.35759999999999997</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.32929999999999998</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.2999</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.26329999999999998</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.24260000000000001</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.2324</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.23760000000000001</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0.24129999999999999</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.2321</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0.21940000000000001</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0.1832</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0.17380000000000001</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0.17730000000000001</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0.18920000000000001</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0.20469999999999999</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>0.18590000000000001</v>
-      </c>
-      <c r="R10" s="2">
-        <v>0.1673</v>
+      <c r="F10" s="1">
+        <v>0.26328978619999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.242627288</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.23242417000000001</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.23762314239999999</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.2412545576</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.2321292975</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.21935918439999999</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.18322236650000001</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.17382754080000001</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.1772625759</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.1891977608</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.20474288769999999</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.1859297228</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0.16727506880000001</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0.1423736665</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0.13766754959999999</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0.14587547219999999</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.29389999999999999</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.25380000000000003</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.16339999999999999</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.13009999999999999</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.10440000000000001</v>
-      </c>
-      <c r="H11" s="2">
-        <v>8.4500000000000006E-2</v>
-      </c>
-      <c r="I11" s="2">
-        <v>6.6199999999999995E-2</v>
-      </c>
-      <c r="J11" s="2">
-        <v>5.0700000000000002E-2</v>
-      </c>
-      <c r="K11" s="2">
-        <v>3.6299999999999999E-2</v>
-      </c>
-      <c r="L11" s="2">
-        <v>2.52E-2</v>
-      </c>
-      <c r="M11" s="2">
-        <v>1.9699999999999999E-2</v>
-      </c>
-      <c r="N11" s="2">
-        <v>1.78E-2</v>
-      </c>
-      <c r="O11" s="2">
-        <v>1.5900000000000001E-2</v>
-      </c>
-      <c r="P11" s="2">
-        <v>1.4200000000000001E-2</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>1.1599999999999999E-2</v>
-      </c>
-      <c r="R11" s="2">
-        <v>1.06E-2</v>
+      <c r="F11" s="1">
+        <v>0.16337974129999999</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.13009966749999999</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.10440006759999999</v>
+      </c>
+      <c r="I11" s="1">
+        <v>8.4525657300000001E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>6.6200310499999998E-2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5.06931942E-2</v>
+      </c>
+      <c r="L11" s="1">
+        <v>3.6307210899999998E-2</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2.5158744E-2</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1.96789359E-2</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1.77784821E-2</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1.58945983E-2</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1.4247231799999999E-2</v>
+      </c>
+      <c r="R11" s="1">
+        <v>1.16063117E-2</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1.0639959399999999E-2</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1.08730939E-2</v>
+      </c>
+      <c r="U11" s="1">
+        <v>1.15015645E-2</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1.0157618199999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>0.64510000000000001</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.57479999999999998</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.53220000000000001</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.4153</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.3715</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.33129999999999998</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.32719999999999999</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.36549999999999999</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.40579999999999999</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0.44440000000000002</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0.4118</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0.44479999999999997</v>
-      </c>
-      <c r="N12" s="2">
-        <v>0.41770000000000002</v>
-      </c>
-      <c r="O12" s="2">
-        <v>0.4007</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0.40179999999999999</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>0.3175</v>
-      </c>
-      <c r="R12" s="2">
-        <v>0.2651</v>
+      <c r="F12" s="1">
+        <v>0.41531027790000002</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.37149472109999998</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.33126424360000001</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.3271811074</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.36550818750000003</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.40581182170000002</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.44442312779999998</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.41179113499999997</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.44477049810000002</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.4176940998</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.40072411130000002</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.40181660079999998</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0.31752852500000001</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0.26505322879999998</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0.22421023840000001</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0.21323881149999999</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0.1362244614</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.3296</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.28549999999999998</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.46010000000000001</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0.63349999999999995</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.59970000000000001</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.42120000000000002</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.36820000000000003</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0.32669999999999999</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.32979999999999998</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0.32969999999999999</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0.26190000000000002</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>0.14729999999999999</v>
-      </c>
-      <c r="R13" s="2">
-        <v>0.1075</v>
+      <c r="F13" s="1">
+        <v>0.46013943289999998</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.53899069779999997</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.63350323320000002</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.59973722620000003</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.42123220750000001</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.36820697930000001</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.32672642299999999</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.32977408000000002</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.329660866</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.31004561619999998</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.26191248880000001</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.20700169169999999</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0.14734001560000001</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0.1075355721</v>
+      </c>
+      <c r="T13" s="1">
+        <v>8.7215216700000001E-2</v>
+      </c>
+      <c r="U13" s="1">
+        <v>9.0053740600000001E-2</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0.13898540649999999</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <v>0.71740000000000004</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.64670000000000005</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.53349999999999997</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.48820000000000002</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.48049999999999998</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.47770000000000001</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.44469999999999998</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.30220000000000002</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0.2631</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0.2167</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0.25690000000000002</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0.27229999999999999</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0.3266</v>
-      </c>
-      <c r="P14" s="2">
-        <v>0.33839999999999998</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0.30570000000000003</v>
-      </c>
-      <c r="R14" s="2">
-        <v>0.25950000000000001</v>
+      <c r="F14" s="1">
+        <v>0.48824478560000001</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.4805199275</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.4776924749</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.44471277510000001</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.39300391169999999</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.3022130596</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.26309155150000002</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0.21673258179999999</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0.25685504809999998</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0.2723351389</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0.32657515079999999</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0.33835293729999999</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0.30567088650000002</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0.25954379259999999</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0.20188107720000001</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.2112739595</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0.29914110430000002</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1">
+        <v>0.30256569989999998</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0.3067050603</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0.30788612440000002</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.35525000499999998</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.39493777159999999</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.39829512049999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" t="s">
-        <v>15</v>
-      </c>
-      <c r="M15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="2">
-        <v>0.63460000000000005</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0.40489999999999998</v>
-      </c>
-      <c r="P15" s="2">
-        <v>0.30259999999999998</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>0.30669999999999997</v>
-      </c>
-      <c r="R15" s="2">
-        <v>0.30790000000000001</v>
+      <c r="F16" s="1">
+        <v>0.3377450649</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.38663281189999998</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.3993659752</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.38164545290000002</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.33474639340000001</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.27919351069999998</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.24365305500000001</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.1919631175</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0.20977115539999999</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0.25161929970000002</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0.27627208380000001</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.31047898229999998</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.28268829359999997</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.26471584190000003</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0.24043311000000001</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.24989998799999999</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.47790868920000001</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.24660000000000001</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.27539999999999998</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.32169999999999999</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.3377</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.3866</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0.39939999999999998</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.38159999999999999</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.3347</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.2792</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0.2437</v>
-      </c>
-      <c r="L16" s="2">
-        <v>0.192</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0.20979999999999999</v>
-      </c>
-      <c r="N16" s="2">
-        <v>0.25159999999999999</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0.27629999999999999</v>
-      </c>
-      <c r="P16" s="2">
-        <v>0.3105</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>0.28270000000000001</v>
-      </c>
-      <c r="R16" s="2">
-        <v>0.26469999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="3"/>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4771,8 +4749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E356A6A6-24A0-42A0-8188-ED9E5DA792BF}">
   <dimension ref="B33:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4781,53 +4759,53 @@
   </cols>
   <sheetData>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M33" s="10"/>
+      <c r="M33" s="9"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" t="s">
         <v>27</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
       </c>
       <c r="L34" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
         <v>32</v>
       </c>
-      <c r="D35" t="s">
+      <c r="L35" t="s">
         <v>33</v>
-      </c>
-      <c r="L35" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
         <v>35</v>
-      </c>
-      <c r="D36" t="s">
-        <v>36</v>
       </c>
       <c r="L36" t="s">
         <v>12</v>
@@ -4835,10 +4813,10 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" t="s">
         <v>37</v>
-      </c>
-      <c r="D37" t="s">
-        <v>38</v>
       </c>
       <c r="L37" t="s">
         <v>1</v>
@@ -4846,10 +4824,10 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
         <v>39</v>
-      </c>
-      <c r="D38" t="s">
-        <v>40</v>
       </c>
       <c r="L38" t="s">
         <v>3</v>
@@ -4857,65 +4835,65 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
         <v>41</v>
-      </c>
-      <c r="D40" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="F44" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="G44" t="s">
         <v>19</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H44" s="7" t="s">
+      <c r="I44" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I44" s="7" t="s">
+      <c r="J44" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D45" s="4"/>
-      <c r="E45" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="6"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J45" s="6"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" s="5"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G47" s="8" t="s">
-        <v>25</v>
+      <c r="G47" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>